<commit_message>
"Order" column in now column 1
Closes #17
</commit_message>
<xml_diff>
--- a/processing/test/20230613-a1r-nc-session3-g_transcript.xlsx
+++ b/processing/test/20230613-a1r-nc-session3-g_transcript.xlsx
@@ -7,7 +7,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20230613-a1r-nc-session3-g_tran" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proposal" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -364,521 +363,520 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Order</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>speaker</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>text</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Has Arguments</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>All Arguments Summarized</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Order</t>
-        </is>
-      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>"2:04"</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>This is Jim in Buffalo New York.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="n">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>"2:09"</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>This is Margaret in Michigan.</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="n">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>48659</v>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>"2:14"</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>Hey, this is Mark in Maine.</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="n">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t>"2:17"</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>It says Aaron from Michigan.</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="n">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="C6" s="4" t="inlineStr">
         <is>
           <t>"2:21"</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>And Kerry from Maryland.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>5</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2" t="n">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>"2:25"</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>Rich from Connecticut. Hopefully you can hear me. Can you hear me?</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>6</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="n">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="C8" s="4" t="inlineStr">
         <is>
           <t>"2:30"</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>Yep. Yep, we can hear you Peter and Wisconsin.</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>7</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="n">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="C9" s="4" t="inlineStr">
         <is>
           <t>"11:00"</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>8</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2" t="n">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="C10" s="4" t="inlineStr">
         <is>
           <t>"11:00"</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>In particular, I like the automatic voter registration. I think that that a lot of time is wasted in in just signing people up to vote. I think the emphasis should be on the actual voting not and we have good records, you know, good motor vehicle records and other records that we can use to create these lists and that's just a starting point for their form.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person likes automatic voter registration.
 2. They believe that a lot of time is wasted on signing people up to vote.
 3. They think the emphasis should be on actual voting.
-4. The person thinks that good motor vehicle records and other records can be used to create lists for voter registration.
-5. They see the automatic voter registration as a starting point for forming the lists.</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>9</v>
+4. They mention that good motor vehicle records and other records can be used to create lists for voter registration.
+5. They suggest that this is just a starting point for voter registration.</t>
+        </is>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="n">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="C11" s="4" t="inlineStr">
         <is>
           <t>"11:00"</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>Voting. I think that's the way to go.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>10</v>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="n">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="C12" s="4" t="inlineStr">
         <is>
           <t>"11:38"</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>I have a difficulty with that. I just think there's too many lists too many ways of cross-contamination and who really determines who an eligible voter is.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>11</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="n">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="C13" s="4" t="inlineStr">
         <is>
           <t>"11:55"</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Everybody is eligible to vote if they're over 21 pretty much, you know, unless you've got laws like you know, not allowing former felons to vote which we'll get to later. But I don't I don't really see the problem there. I mean, if there's worries about fraud that can be handled in the election process, we I think we waste a lot of time if we require people to</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>12</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="n">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B14" s="4" t="inlineStr">
+      <c r="C14" s="4" t="inlineStr">
         <is>
           <t>"11:55"</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>to keep registering to vote as a separate.</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>13</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="n">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B15" s="4" t="inlineStr">
+      <c r="C15" s="4" t="inlineStr">
         <is>
           <t>"12:31"</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>My question would be, how do you think we can handle the fraud in the election process?</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1. Identify the types of fraud that can occur in an election process.
-2. Implement voter identification measures to prevent voter impersonation.
-3. Use paper trails for votes to allow for recounts and audits.
-4. Train poll workers to recognize and prevent fraudulent activities.
-5. Strengthen laws and penalties for election fraud.
-6. Increase transparency in the election process.
-7. Use technology to monitor and detect unusual voting patterns.
-8. Promote public education about the importance of fair and honest elections.
-9. Encourage citizen participation in election monitoring and reporting suspicious activities.</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>14</v>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. Firstly, implementing a secure voter identification system to prevent voter impersonation.
+2. Secondly, ensuring the accuracy of voter registration lists to prevent duplicate or fraudulent registrations.
+3. Thirdly, monitoring and regulating campaign financing to prevent illegal or unethical influence.
+4. Additionally, establishing post-election audits to verify the results and detect any discrepancies.
+5. Furthermore, enacting strict penalties for election fraud to deter potential violators.
+6. Lastly, promoting transparency and public participation in the election process to increase accountability and trust.</t>
+        </is>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="n">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B16" s="4" t="inlineStr">
+      <c r="C16" s="4" t="inlineStr">
         <is>
           <t>"12:40"</t>
         </is>
       </c>
-      <c r="C16" s="2" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
         <is>
           <t>How do we handle it in the registration process?</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>15</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="n">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="C17" s="4" t="inlineStr">
         <is>
           <t>"12:53"</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>I agree with Peter. I think it's a would be more more uniform to just do it that way, and give people the option to opt-out certain animal with the mechanism would be to regulate, you know, who's koala a qualified voter or not. But</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>16</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="n">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="C18" s="4" t="inlineStr">
         <is>
           <t>"13:12"</t>
         </is>
       </c>
-      <c r="C18" s="2" t="inlineStr">
+      <c r="D18" s="2" t="inlineStr">
         <is>
           <t>I'm not against the proposal, I just see a lot of hurdles to really implementing it.</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person does not oppose the proposal.
 2. There are many challenges or obstacles to implementing the proposal.</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="n">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
         <v>9671</v>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="C19" s="4" t="inlineStr">
         <is>
           <t>"13:26"</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>18</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="n">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="n">
         <v>9671</v>
       </c>
-      <c r="B20" s="4" t="inlineStr">
+      <c r="C20" s="4" t="inlineStr">
         <is>
           <t>"13:26"</t>
         </is>
       </c>
-      <c r="C20" s="2" t="inlineStr">
+      <c r="D20" s="2" t="inlineStr">
         <is>
           <t>I agree with Margaret, I think it'll be just a lot of to go through and then plus you</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> have to do the analysis afterwards. Also, I don't think we have enough information to make an informed decision. Plus, there are other factors to consider, like the time and resources it would take to implement the change.
-1. There is agreement that going through with the proposed action would require a lot of effort.
-2. Analysis would be required after the action is taken.
-3. There is not enough information to make an informed decision.
-4. The time and resources required to implement the change are factors that need to be considered.</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>19</v>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> have to do the analysis afterwards. Also, I don't think we have the necessary data to make informed decisions. Here are the points I agree with Margaret on:
+1. The process of going through all the data will be time-consuming.
+2. Analysis of the data will be required after collecting it.
+3. The necessary data for making informed decisions is currently lacking.</t>
+        </is>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="n">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B21" s="4" t="inlineStr">
+      <c r="C21" s="4" t="inlineStr">
         <is>
           <t>"14:13"</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>One of the other things was gloating online which I, I certainly think that that's probably not workable. I don't know what other people think about that, but I would be against</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text discusses the issue of gloating online.
 2. The author expresses their personal opinion that gloating online is not productive or workable.
@@ -886,30 +884,30 @@
 4. The author states that they would be against gloating online.</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="n">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B22" s="4" t="inlineStr">
+      <c r="C22" s="4" t="inlineStr">
         <is>
           <t>"14:29"</t>
         </is>
       </c>
-      <c r="C22" s="2" t="inlineStr">
+      <c r="D22" s="2" t="inlineStr">
         <is>
           <t>I agree. I think that right now, there's just too many possibilities of people not knowing how to use the computer system to vote correctly, fraud, multiple voting. I think it's just too difficult.</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person believes that there are currently too many possibilities of people not knowing how to use the computer system to vote correctly.
 2. The person is concerned about the possibility of fraud.
@@ -917,122 +915,122 @@
 4. The person thinks that the computer system for voting is too difficult to use.</t>
         </is>
       </c>
-      <c r="F22" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="23" ht="12.5" customHeight="1">
-      <c r="A23" s="2" t="n">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B23" s="4" t="inlineStr">
+      <c r="C23" s="4" t="inlineStr">
         <is>
           <t>"14:46"</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>I think that the proposal is for registering to vote online, I don't think that they're necessarily proposing that we actually do the voting online itself. As far as that goes, I think Most states have, you know, allow you to do your driver's license to renew your drivers license and vehicles and stuff online. So if they can get that figured out, I think that they could tag the</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>22</v>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="24" ht="12.5" customHeight="1">
-      <c r="A24" s="2" t="n">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B24" s="4" t="inlineStr">
+      <c r="C24" s="4" t="inlineStr">
         <is>
           <t>"14:46"</t>
         </is>
       </c>
-      <c r="C24" s="2" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>Voter registration online as well as long as you have the proper IDs and all that kind of stuff.</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>23</v>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="25" ht="12.5" customHeight="1">
-      <c r="A25" s="2" t="n">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="C25" s="4" t="inlineStr">
         <is>
           <t>"15:21"</t>
         </is>
       </c>
-      <c r="C25" s="2" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>No I agree with Kerry. I think that you know the question here is can the register to vote online? And that's something that I think should be allowed, certainly not as the only option, but an additional option because in, you know, today's world is going to computers and there's no stopping that and you know I think to just not allow that as an option, I think is denying a basic</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>24</v>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="26" ht="12.5" customHeight="1">
-      <c r="A26" s="2" t="n">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B26" s="4" t="inlineStr">
+      <c r="C26" s="4" t="inlineStr">
         <is>
           <t>"15:21"</t>
         </is>
       </c>
-      <c r="C26" s="2" t="inlineStr">
+      <c r="D26" s="2" t="inlineStr">
         <is>
           <t>Practice that just makes sense in today's world.</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>25</v>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="27" ht="12.5" customHeight="1">
-      <c r="A27" s="2" t="n">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="C27" s="4" t="inlineStr">
         <is>
           <t>"15:53"</t>
         </is>
       </c>
-      <c r="C27" s="2" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>Yeah, I agree. I'm sorry, I misread that in the other thing is allowing registering to vote on Election Day. We've had that in Wisconsin for a long time. I don't think there's any problem with that. I don't see a need for a pre-registration but I think the automat taking like the motor vehicle list makes the most sense because you've already identified people and I just don't see a problem.</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with a previous statement.
 2. The speaker apologizes for a previous misreading.
@@ -1043,30 +1041,30 @@
 7. The speaker sees no problems with using the motor vehicle list for registration.</t>
         </is>
       </c>
-      <c r="F27" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="28" ht="12.5" customHeight="1">
-      <c r="A28" s="2" t="n">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B28" s="4" t="inlineStr">
+      <c r="C28" s="4" t="inlineStr">
         <is>
           <t>"16:25"</t>
         </is>
       </c>
-      <c r="C28" s="2" t="inlineStr">
+      <c r="D28" s="2" t="inlineStr">
         <is>
           <t>I agree. I think I'll registering online is fine and also the vehicle motor list and I think that would cover most people. However, there are a lot of people who do not drive so you'd have to try to figure out how to get those people. The other question. I have regarding this registration getting there by the date of the election versus I know in our state, we they allowed for time after the election.</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. It is agreed to register online for the election.
 2. Registering the vehicle motor list is also recommended.
@@ -1076,53 +1074,53 @@
 6. It is mentioned that in the speaker's state, registration is allowed after the election.</t>
         </is>
       </c>
-      <c r="F28" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="29" ht="12.5" customHeight="1">
-      <c r="A29" s="2" t="n">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B29" s="4" t="inlineStr">
+      <c r="C29" s="4" t="inlineStr">
         <is>
           <t>"16:25"</t>
         </is>
       </c>
-      <c r="C29" s="2" t="inlineStr">
+      <c r="D29" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> So, how do we feel about that?</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>28</v>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="30" ht="12.5" customHeight="1">
-      <c r="A30" s="2" t="n">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B30" s="4" t="inlineStr">
+      <c r="C30" s="4" t="inlineStr">
         <is>
           <t>"19:03"</t>
         </is>
       </c>
-      <c r="C30" s="2" t="inlineStr">
+      <c r="D30" s="2" t="inlineStr">
         <is>
           <t>I apologize. I jumped ahead when I proposed my question about receiving, ballots on the day of the election versus waiting.</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text discusses a point about election procedures.
 2. The author apologizes for bringing up a question about receiving ballots on the day of the election versus waiting.
@@ -1130,30 +1128,30 @@
 4. However, the text does not provide context or details about that previous discussion.</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="31" ht="12.5" customHeight="1">
-      <c r="A31" s="2" t="n">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B31" s="4" t="inlineStr">
+      <c r="C31" s="4" t="inlineStr">
         <is>
           <t>"19:28"</t>
         </is>
       </c>
-      <c r="C31" s="2" t="inlineStr">
+      <c r="D31" s="2" t="inlineStr">
         <is>
           <t>I know this might not be the most popular vote, but I believe in one of these, in the one I believe in is that voters should vote in person on Election Day unless medically, or health related reasons, prohibit them from doing that. I think that that's some I don't like the idea of mail-in ballots. I think it's a mess. It causes too many problems and it's just, it's unreliable and too easy to be manipulated.</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker believes that voters should vote in person on Election Day.
 2. The speaker thinks that mail-in ballots are not a good idea.
@@ -1163,148 +1161,139 @@
 6. The speaker does not like the idea of mail-in ballots for health or medical reasons.</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="32" ht="12.5" customHeight="1">
-      <c r="A32" s="2" t="n">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B32" s="4" t="inlineStr">
+      <c r="C32" s="4" t="inlineStr">
         <is>
           <t>"19:56"</t>
         </is>
       </c>
-      <c r="C32" s="2" t="inlineStr">
+      <c r="D32" s="2" t="inlineStr">
         <is>
           <t>Yeah, I completely disagree with that. I think I vote by mail has worked very well. And a lot of places. There are some states that do all their elections by mail and they have not really had problems. I think, I think Oregon does that. I think maybe Utah does that. And we certainly have have it available in Wisconsin. So I'm I'm really all four</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1. The text author disagrees with the statement that voting by mail has not worked well.
-2. The text author believes that voting by mail has worked very well in many places.
-3. There are some states that conduct all their elections by mail and have not encountered significant problems.
-4. Oregon and Utah are mentioned as examples of states that conduct all their elections by mail.
-5. Voting by mail is available in Wisconsin.
-6. The text author supports the use of voting by mail.</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>31</v>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="33" ht="12.5" customHeight="1">
-      <c r="A33" s="2" t="n">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B33" s="4" t="inlineStr">
+      <c r="C33" s="4" t="inlineStr">
         <is>
           <t>"19:56"</t>
         </is>
       </c>
-      <c r="C33" s="2" t="inlineStr">
+      <c r="D33" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Voting by mail you, I just tell you I don't think we've had a problem with it.</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>32</v>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="34" ht="12.5" customHeight="1">
-      <c r="A34" s="2" t="n">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B34" s="4" t="inlineStr">
+      <c r="C34" s="4" t="inlineStr">
         <is>
           <t>"20:33"</t>
         </is>
       </c>
-      <c r="C34" s="2" t="inlineStr">
+      <c r="D34" s="2" t="inlineStr">
         <is>
           <t>I don't like that by now. I think people should be required to be in person. I also think that people should be required to show ID when they vote, which is something that you can't ask them to do with the vote by mail. However, I think there should be a couple either exceptions to people that are allowed to vote by mail because like, I know my, my son is still in college and it while it's still within the state. It's three and a half hours away. He can't make it back.</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E34" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person expresses dislike towards something.
 2. They believe people should be required to vote in person.
-3. The person thinks that voters should be required to show ID when voting, which is not possible with mail-in voting.
+3. The person thinks voters should be required to show ID when voting, which is not possible with mail-in voting.
 4. However, they think there should be exceptions for people allowed to vote by mail.
-5. One example of such an exception is for the person's son, who is in college and cannot make it back to vote in person.</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
-        <v>33</v>
+5. One example of such an exception is a person's son, who is still in college and resides three and a half hours away from his voting location.
+6. The son is unable to return to vote in person.</t>
+        </is>
       </c>
     </row>
     <row r="35" ht="12.5" customHeight="1">
-      <c r="A35" s="2" t="n">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B35" s="4" t="inlineStr">
+      <c r="C35" s="4" t="inlineStr">
         <is>
           <t>"20:33"</t>
         </is>
       </c>
-      <c r="C35" s="2" t="inlineStr">
+      <c r="D35" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Back to, to vote on Election Day. So he kind of has to do by mail</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E35" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. A person, named John, plans to go out of town for vacation.
 2. John's vacation will coincide with the Election Day.
 3. Therefore, John needs to vote by mail instead of going to a polling place on Election Day.</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>34</v>
-      </c>
     </row>
     <row r="36" ht="12.5" customHeight="1">
-      <c r="A36" s="2" t="n">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B36" s="4" t="inlineStr">
+      <c r="C36" s="4" t="inlineStr">
         <is>
           <t>"21:09"</t>
         </is>
       </c>
-      <c r="C36" s="2" t="inlineStr">
+      <c r="D36" s="2" t="inlineStr">
         <is>
           <t>Yeah, I'm fine with voting by mail. I mean, obviously this last election there are tons of audits done and everything checked out there was no evidence of fraud. I can also say I'm very much in favor of early voting because I have lived in a small town of just 2,000 people in Michigan. That I also lived in</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E36" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The writer is in favor of voting by mail.
 2. In the last election, there were numerous audits done, and no evidence of fraud was found.
@@ -1312,30 +1301,30 @@
 4. The writer has lived in a small town of 2,000 people in Michigan.</t>
         </is>
       </c>
-      <c r="F36" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="37" ht="12.5" customHeight="1">
-      <c r="A37" s="2" t="n">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B37" s="4" t="inlineStr">
+      <c r="C37" s="4" t="inlineStr">
         <is>
           <t>"21:09"</t>
         </is>
       </c>
-      <c r="C37" s="2" t="inlineStr">
+      <c r="D37" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> In Miami, Florida. And I did early voting in Miami and I had to wait for hours to do early voting. If you wait the day of sometimes, it might be 12-hour. Wait,</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E37" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The individual voted in Miami, Florida.
 2. They participated in early voting in Miami.
@@ -1343,30 +1332,30 @@
 4. If one waits until the day of the election, the wait time could be up to 12 hours.</t>
         </is>
       </c>
-      <c r="F37" t="n">
-        <v>36</v>
-      </c>
     </row>
     <row r="38" ht="12.5" customHeight="1">
-      <c r="A38" s="2" t="n">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B38" s="4" t="inlineStr">
+      <c r="C38" s="4" t="inlineStr">
         <is>
           <t>"22:02"</t>
         </is>
       </c>
-      <c r="C38" s="2" t="inlineStr">
+      <c r="D38" s="2" t="inlineStr">
         <is>
           <t>I think we have to think of the military and people who are out of the country, for example, on business. I think those should individuals should be allowed to vote by mail. In addition, to elderly people above a certain age, the way it is now. So I'm all in favor for male voting. And I have no problem with early voting either as long as it's a reasonable amount of time within the election day.</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The military and people who are outside of the country for work should be allowed to vote by mail.
 2. Elderly people, beyond a certain age, should continue to be allowed to vote in the way they do now (which may imply voting by mail for some of them).
@@ -1374,235 +1363,235 @@
 4. The speaker has no issue with early voting, as long as it is within a reasonable timeframe relative to the election day.</t>
         </is>
       </c>
-      <c r="F38" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="39" ht="12.5" customHeight="1">
-      <c r="A39" s="2" t="n">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B39" s="4" t="inlineStr">
+      <c r="C39" s="4" t="inlineStr">
         <is>
           <t>"22:39"</t>
         </is>
       </c>
-      <c r="C39" s="2" t="inlineStr">
+      <c r="D39" s="2" t="inlineStr">
         <is>
           <t>What do you think about the video cameras at the voting site?</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>38</v>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="40" ht="12.5" customHeight="1">
-      <c r="A40" s="2" t="n">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B40" s="4" t="inlineStr">
+      <c r="C40" s="4" t="inlineStr">
         <is>
           <t>"22:50"</t>
         </is>
       </c>
-      <c r="C40" s="2" t="inlineStr">
+      <c r="D40" s="2" t="inlineStr">
         <is>
           <t>I don't see a problem with that, I know and some cases, I think the last election they had police officers monitoring the boxes but I don't see any problem having a camera there for security. Keep everything legit.</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>39</v>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="41" ht="12.5" customHeight="1">
-      <c r="A41" s="2" t="n">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B41" s="4" t="inlineStr">
+      <c r="C41" s="4" t="inlineStr">
         <is>
           <t>"23:16"</t>
         </is>
       </c>
-      <c r="C41" s="2" t="inlineStr">
+      <c r="D41" s="2" t="inlineStr">
         <is>
           <t>I don't have a problem with the video cameras either as long as everybody knows about it, I do have a problem with a paper record where the voter has to verify and and then put it in. I think, just adding a layer, a confusing layer to the voting process</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person mentioned does not have an issue with video cameras at polling stations, as long as their presence is known to everyone.
 2. They have a concern with a system that involves a paper record which the voter has to verify and then submit.
 3. They believe that this additional layer could make the voting process more confusing.</t>
         </is>
       </c>
-      <c r="F41" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="42" ht="12.5" customHeight="1">
-      <c r="A42" s="2" t="n">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B42" s="4" t="inlineStr">
+      <c r="C42" s="4" t="inlineStr">
         <is>
           <t>"25:46"</t>
         </is>
       </c>
-      <c r="C42" s="2" t="inlineStr">
+      <c r="D42" s="2" t="inlineStr">
         <is>
           <t>I would be for uniform Across the Nation because otherwise, you can do get situations where in certain States, they make it more difficult for people in large cities to vote. And I can say that as somebody who lived in Florida and when I lived in Miami, you know, like I said, even doing early voting, I waited my wife and I waited for hours to vote. And then later,</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>41</v>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="43" ht="12.5" customHeight="1">
-      <c r="A43" s="2" t="n">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B43" s="4" t="inlineStr">
+      <c r="C43" s="4" t="inlineStr">
         <is>
           <t>"25:46"</t>
         </is>
       </c>
-      <c r="C43" s="2" t="inlineStr">
+      <c r="D43" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Iran. They did things like quietly removed bathrooms out. Hoses from where people were boating basically, to try to discourage people from coming and voting.</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>42</v>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="44" ht="12.5" customHeight="1">
-      <c r="A44" s="2" t="n">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B44" s="4" t="inlineStr">
+      <c r="C44" s="4" t="inlineStr">
         <is>
           <t>"26:36"</t>
         </is>
       </c>
-      <c r="C44" s="2" t="inlineStr">
+      <c r="D44" s="2" t="inlineStr">
         <is>
           <t>I'm torn on this one because they're, like I said, there are times when certain areas do things that are not acceptable, but on the other hand, I fear too much Federal level control and would that allow states to try new methods new techniques for voting like some of the different states have tried. So I'm sort of torn out on this one.</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>43</v>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="45" ht="12.5" customHeight="1">
-      <c r="A45" s="2" t="n">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B45" s="4" t="inlineStr">
+      <c r="C45" s="4" t="inlineStr">
         <is>
           <t>"27:07"</t>
         </is>
       </c>
-      <c r="C45" s="2" t="inlineStr">
+      <c r="D45" s="2" t="inlineStr">
         <is>
           <t>I think you could set like standards, you know, national standards without being too terribly specific, so that implemented so that experimentation could be allowed for in certain areas. But you wouldn't have to, you know, you would have to make very, very specific rules. Just overall standards for voting.</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. It is suggested to establish national standards for voting.
 2. These standards should not be too specific, to allow for experimentation in certain areas.
 3. Specific rules should be made for overall standards of voting.</t>
         </is>
       </c>
-      <c r="F45" t="n">
-        <v>44</v>
-      </c>
     </row>
     <row r="46" ht="12.5" customHeight="1">
-      <c r="A46" s="2" t="n">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="n">
         <v>48659</v>
       </c>
-      <c r="B46" s="4" t="inlineStr">
+      <c r="C46" s="4" t="inlineStr">
         <is>
           <t>"27:37"</t>
         </is>
       </c>
-      <c r="C46" s="2" t="inlineStr">
+      <c r="D46" s="2" t="inlineStr">
         <is>
           <t>yeah, kind of along the lines with Peter was saying, I don't necessarily think that should be uniform, standards Nationwide, but I think there should be minimum standards for each of the different aspects of mail-in voting early finger on Election Day voting that at least keep working minimum standards</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with Peter's viewpoint.
 2. The speaker does not believe that voting standards should be uniform nationwide.
 3. The speaker thinks that there should be minimum standards for different aspects of mail-in voting, early voting, and Election Day voting.</t>
         </is>
       </c>
-      <c r="F46" t="n">
-        <v>45</v>
-      </c>
     </row>
     <row r="47" ht="12.5" customHeight="1">
-      <c r="A47" s="2" t="n">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="n">
         <v>48660</v>
       </c>
-      <c r="B47" s="4" t="inlineStr">
+      <c r="C47" s="4" t="inlineStr">
         <is>
           <t>"28:01"</t>
         </is>
       </c>
-      <c r="C47" s="2" t="inlineStr">
+      <c r="D47" s="2" t="inlineStr">
         <is>
           <t>Yeah, I agree with both Peter and Mark one of those standards would be individuals having to produce a government-issued ID at the time of voting to make sure that people are actually in fact eligible. So I think that would be one of the basic standards for</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The use of government-issued IDs at voting locations to verify the eligibility of individuals.
 2. This standard is supported by both Peter and Mark.
@@ -1610,194 +1599,194 @@
 4. The standard is a basic requirement for a secure and fair voting process.</t>
         </is>
       </c>
-      <c r="F47" t="n">
-        <v>46</v>
-      </c>
     </row>
     <row r="48" ht="12.5" customHeight="1">
-      <c r="A48" s="2" t="n">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="n">
         <v>48660</v>
       </c>
-      <c r="B48" s="4" t="inlineStr">
+      <c r="C48" s="4" t="inlineStr">
         <is>
           <t>"28:01"</t>
         </is>
       </c>
-      <c r="C48" s="2" t="inlineStr">
+      <c r="D48" s="2" t="inlineStr">
         <is>
           <t>voting.</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F48" t="n">
-        <v>47</v>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="49" ht="12.5" customHeight="1">
-      <c r="A49" s="2" t="n">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="n">
         <v>48660</v>
       </c>
-      <c r="B49" s="4" t="inlineStr">
+      <c r="C49" s="4" t="inlineStr">
         <is>
           <t>"28:01"</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
-        <v>48</v>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="50" ht="12.5" customHeight="1">
-      <c r="A50" s="2" t="n">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B50" s="4" t="inlineStr">
+      <c r="C50" s="4" t="inlineStr">
         <is>
           <t>"28:27"</t>
         </is>
       </c>
-      <c r="C50" s="2" t="inlineStr">
+      <c r="D50" s="2" t="inlineStr">
         <is>
           <t>As far as ideas go, I just I'm okay with IDs having to present an 80s, but I do think that there should be a variety of ideas accepted, not all ideas are stupid. There are there have been cases? I think maybe in Texas, were they had, they were allowing like hunting licenses but not student IDs. And you know what was behind that I wonder?</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1. The speaker is open to the idea of IDs having an 80s style.
-2. The speaker believes that a variety of ideas should be accepted.
-3. The speaker mentions an example of Texas allowing hunting licenses but not student IDs.
-4. The speaker wonders about the reasoning behind this example.</t>
-        </is>
-      </c>
-      <c r="F50" t="n">
-        <v>49</v>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is open to the idea of IDs requiring a specific design from the 1980s.
+2. The speaker believes that a variety of ideas should be accepted, and not all ideas are bad.
+3. There is a reference to a potential case in Texas where hunting licenses were allowed, but not student IDs.
+4. The speaker wonders about the motivation behind this hypothetical situation.</t>
+        </is>
       </c>
     </row>
     <row r="51" ht="12.5" customHeight="1">
-      <c r="A51" s="2" t="n">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B51" s="4" t="inlineStr">
+      <c r="C51" s="4" t="inlineStr">
         <is>
           <t>"29:03"</t>
         </is>
       </c>
-      <c r="C51" s="2" t="inlineStr">
+      <c r="D51" s="2" t="inlineStr">
         <is>
           <t>That's interesting, hunting licenses versus student IDs. I like the idea of basic standardized requirements and then within that each state could work out what works best for them.</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F51" t="n">
-        <v>50</v>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="52" ht="12.5" customHeight="1">
-      <c r="A52" s="2" t="n">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B52" s="4" t="inlineStr">
+      <c r="C52" s="4" t="inlineStr">
         <is>
           <t>"29:23"</t>
         </is>
       </c>
-      <c r="C52" s="2" t="inlineStr">
+      <c r="D52" s="2" t="inlineStr">
         <is>
           <t>I agree standardized requirements would work as far as the IDS, I'm not sure maybe driver's license and then there was a don't drive a state issued ID. I'm not sure how regulated other licenses are going to be a hunting license. If that's something that's issued at a</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F52" t="n">
-        <v>51</v>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="53" ht="12.5" customHeight="1">
-      <c r="A53" s="2" t="n">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B53" s="4" t="inlineStr">
+      <c r="C53" s="4" t="inlineStr">
         <is>
           <t>"29:23"</t>
         </is>
       </c>
-      <c r="C53" s="2" t="inlineStr">
+      <c r="D53" s="2" t="inlineStr">
         <is>
           <t>Sporting good store or something like that is.</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F53" t="n">
-        <v>52</v>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="54" ht="12.5" customHeight="1">
-      <c r="A54" s="2" t="n">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B54" s="4" t="inlineStr">
+      <c r="C54" s="4" t="inlineStr">
         <is>
           <t>"29:23"</t>
         </is>
       </c>
-      <c r="C54" s="2" t="inlineStr">
+      <c r="D54" s="2" t="inlineStr">
         <is>
           <t>Is scrutinized.</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F54" t="n">
-        <v>53</v>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="55" ht="12.5" customHeight="1">
-      <c r="A55" s="2" t="n">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="n">
         <v>9671</v>
       </c>
-      <c r="B55" s="4" t="inlineStr">
+      <c r="C55" s="4" t="inlineStr">
         <is>
           <t>"29:47"</t>
         </is>
       </c>
-      <c r="C55" s="2" t="inlineStr">
+      <c r="D55" s="2" t="inlineStr">
         <is>
           <t>Each state Most states have my line of Georgia for sure. Does, they'll give you a state issued ID for free just so you can vote and that would cut a lot of the problem with IDs down. So it'd be a state issued ID or a driver's license.</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E55" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Most states require voters to show an ID
 2. Georgia is an example of a state that requires an ID to vote
@@ -1806,224 +1795,224 @@
 5. This can help reduce problems with ID requirements for voting.</t>
         </is>
       </c>
-      <c r="F55" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="56" ht="12.5" customHeight="1">
-      <c r="A56" s="2" t="n">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B56" s="4" t="inlineStr">
+      <c r="C56" s="4" t="inlineStr">
         <is>
           <t>"30:11"</t>
         </is>
       </c>
-      <c r="C56" s="2" t="inlineStr">
+      <c r="D56" s="2" t="inlineStr">
         <is>
           <t>That's what Michigan does. Also, if you don't drive, you can go in and get a state ID, which is used for identification and almost every venue that will looks up to driver's license.</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F56" t="n">
-        <v>55</v>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="57" ht="12.5" customHeight="1">
-      <c r="A57" s="2" t="n">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B57" s="4" t="inlineStr">
+      <c r="C57" s="4" t="inlineStr">
         <is>
           <t>"30:55"</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F57" t="n">
-        <v>56</v>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="58" ht="12.5" customHeight="1">
-      <c r="A58" s="2" t="n">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B58" s="4" t="inlineStr">
+      <c r="C58" s="4" t="inlineStr">
         <is>
           <t>"30:55"</t>
         </is>
       </c>
-      <c r="C58" s="2" t="inlineStr">
+      <c r="D58" s="2" t="inlineStr">
         <is>
           <t>I think once a person has paid their debt to society, they ought to be able to vote. There's no question in my mind about that, I think it's terrible. That some states are not allowing former felons to</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F58" t="n">
-        <v>57</v>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="59" ht="12.5" customHeight="1">
-      <c r="A59" s="2" t="n">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B59" s="4" t="inlineStr">
+      <c r="C59" s="4" t="inlineStr">
         <is>
           <t>"31:14"</t>
         </is>
       </c>
-      <c r="C59" s="2" t="inlineStr">
+      <c r="D59" s="2" t="inlineStr">
         <is>
           <t>I can't, I completely agree with Peter. I think you paid your debt to society. You paid the penalty your time. Now you should be able to vote. Again, is one of your rights that you earned back by doing your time.</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F59" t="n">
-        <v>58</v>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="60" ht="12.5" customHeight="1">
-      <c r="A60" s="2" t="n">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="n">
         <v>48660</v>
       </c>
-      <c r="B60" s="4" t="inlineStr">
+      <c r="C60" s="4" t="inlineStr">
         <is>
           <t>"31:29"</t>
         </is>
       </c>
-      <c r="C60" s="2" t="inlineStr">
+      <c r="D60" s="2" t="inlineStr">
         <is>
           <t>I think the only exception to that would be if the individual was convicted and sentenced to prison. Because of voter fraud, then probably not in that case. But otherwise if we are saying that they are rehabilitated and can reenter Society, then they have a right to participate in the process of living in society. And that includes voting.</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E60" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 1. If an individual has been convicted and sentenced to prison due to voter fraud, they probably should not be allowed to vote.
-2. Those who have been rehabilitated and can reenter society should be able to participate in the process of living in society, including voting.</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
-        <v>59</v>
+2. Those who have been rehabilitated and can re-enter society have the right to participate in the process of living in society, including voting.</t>
+        </is>
       </c>
     </row>
     <row r="61" ht="12.5" customHeight="1">
-      <c r="A61" s="2" t="n">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B61" s="4" t="inlineStr">
+      <c r="C61" s="4" t="inlineStr">
         <is>
           <t>"31:57"</t>
         </is>
       </c>
-      <c r="C61" s="2" t="inlineStr">
+      <c r="D61" s="2" t="inlineStr">
         <is>
           <t>I agree somebody that's served their time and rehabilitated, you know, learning that right back as well.</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F61" t="n">
-        <v>60</v>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="62" ht="12.5" customHeight="1">
-      <c r="A62" s="2" t="n">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="n">
         <v>9671</v>
       </c>
-      <c r="B62" s="4" t="inlineStr">
+      <c r="C62" s="4" t="inlineStr">
         <is>
           <t>"32:05"</t>
         </is>
       </c>
-      <c r="C62" s="2" t="inlineStr">
+      <c r="D62" s="2" t="inlineStr">
         <is>
           <t>I kind of disagree, I think it should go back a case-by-case bright basis. I think you should have to make some kind of requirement to do that because I mean, there's some people that I wouldn't care if they breathe much less vote.</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F62" t="n">
-        <v>61</v>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="63" ht="12.5" customHeight="1">
-      <c r="A63" s="2" t="n">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B63" s="4" t="inlineStr">
+      <c r="C63" s="4" t="inlineStr">
         <is>
           <t>"32:21"</t>
         </is>
       </c>
-      <c r="C63" s="2" t="inlineStr">
+      <c r="D63" s="2" t="inlineStr">
         <is>
           <t>I don't like the word in on some of the things the things I've seen about it saying, like, like where it says non incarcerated, I think they have to completely finish their their sentence, including any parole, I need anything like that. And so, just the fact that they're not in jail anymore, I don't think should be enough. I think they need to finish parole. And, and then at that point, I think it's probably. Okay.</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E63" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker does not like the use of the word "in" in certain contexts.
 2. They have concerns about the status of individuals who have served jail time.
 3. The speaker believes that these individuals should completely finish their sentence, including any parole.
 4. The mere fact that someone is not in jail anymore is not sufficient, according to the speaker.
-5. The speaker thinks that only after finishing parole should the individual be considered as having served their sentence.</t>
-        </is>
-      </c>
-      <c r="F63" t="n">
-        <v>62</v>
+5. The speaker thinks that only after finishing parole should the individual be considered for any further actions.</t>
+        </is>
       </c>
     </row>
     <row r="64" ht="12.5" customHeight="1">
-      <c r="A64" s="2" t="n">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B64" s="4" t="inlineStr">
+      <c r="C64" s="4" t="inlineStr">
         <is>
           <t>"32:49"</t>
         </is>
       </c>
-      <c r="C64" s="2" t="inlineStr">
+      <c r="D64" s="2" t="inlineStr">
         <is>
           <t>I took my thoughts were along those lines. Also finish the time that they've been sentenced to, in then parole, I think as a time where they prove that they come back into society and I think once the parole has been finished, then they should be eligible to vote.</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E64" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker's thoughts align with the listener's viewpoint.
 2. The speaker believes that a person's sentence should include a parole period.
@@ -2031,48 +2020,48 @@
 4. Once parole is completed, the speaker thinks the person should be eligible to vote.</t>
         </is>
       </c>
-      <c r="F64" t="n">
-        <v>63</v>
-      </c>
     </row>
     <row r="65" ht="12.5" customHeight="1">
-      <c r="A65" s="2" t="n">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B65" s="4" t="inlineStr">
+      <c r="C65" s="4" t="inlineStr">
         <is>
           <t>"34:35"</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F65" t="n">
-        <v>64</v>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="66" ht="12.5" customHeight="1">
-      <c r="A66" s="2" t="n">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B66" s="4" t="inlineStr">
+      <c r="C66" s="4" t="inlineStr">
         <is>
           <t>"34:35"</t>
         </is>
       </c>
-      <c r="C66" s="2" t="inlineStr">
+      <c r="D66" s="2" t="inlineStr">
         <is>
           <t>I am very much against having people just random people challenging voters. I think that's intimidating, and I don't think that should be done. I think that, you know, having voter ID and all that sort of thing, you know, is the way of legitimizing Voters, and not having just people show up at the polls and and challenging people that they, they think.</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E66" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker is against having random people challenging voters.
 2. The speaker finds this practice intimidating.
@@ -2080,116 +2069,114 @@
 4. The speaker is not in favor of people showing up at the polls and challenging others they think are not legitimate voters.</t>
         </is>
       </c>
-      <c r="F66" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="67" ht="12.5" customHeight="1">
-      <c r="A67" s="2" t="n">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B67" s="4" t="inlineStr">
+      <c r="C67" s="4" t="inlineStr">
         <is>
           <t>"34:35"</t>
         </is>
       </c>
-      <c r="C67" s="2" t="inlineStr">
+      <c r="D67" s="2" t="inlineStr">
         <is>
           <t>Might have voted the way they didn't like or whatever. I just think that's a terrible idea.</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F67" t="n">
-        <v>66</v>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="68" ht="12.5" customHeight="1">
-      <c r="A68" s="2" t="n">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B68" s="4" t="inlineStr">
+      <c r="C68" s="4" t="inlineStr">
         <is>
           <t>"35:11"</t>
         </is>
       </c>
-      <c r="C68" s="2" t="inlineStr">
+      <c r="D68" s="2" t="inlineStr">
         <is>
           <t>I agree. I agree with that. I think, like you said, it's intimidating and unnecessary and I thought we already had criminal penalties for misleading, citizens, etc, etc. I do like the idea of random Audits and different voting areas throughout the election process. I think that would help answer some questions of people being suspicious of the process.</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1. The speaker agrees with the previous statement.
-2. They find the subject matter intimidating and unnecessary.
-3. The speaker believes there are already criminal penalties for misleading citizens.
-4. The speaker appreciates the idea of random audits during the election process.
-5. They also like the idea of having different voting areas throughout the election process.
-6. The speaker thinks these ideas would help address suspicions about the process.</t>
-        </is>
-      </c>
-      <c r="F68" t="n">
-        <v>67</v>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The reader agrees that the process described is intimidating and unnecessary.
+2. The reader thinks that criminal penalties for misleading citizens already exist.
+3. The reader supports the idea of random audits during the election process.
+4. The reader believes that different voting areas throughout the election process would help address suspicions of the public regarding the process.</t>
+        </is>
       </c>
     </row>
     <row r="69" ht="12.5" customHeight="1">
-      <c r="A69" s="2" t="n">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B69" s="4" t="inlineStr">
+      <c r="C69" s="4" t="inlineStr">
         <is>
           <t>"35:42"</t>
         </is>
       </c>
-      <c r="C69" s="2" t="inlineStr">
+      <c r="D69" s="2" t="inlineStr">
         <is>
           <t>Yeah, I'm very much against challenging voters. It's as to whether they're eligible or not, that's just intimidation.</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E69" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person is against challenging voters.
 2. They believe that checking eligibility is separate from challenging voters.
 3. They view challenging voters as a form of intimidation.</t>
         </is>
       </c>
-      <c r="F69" t="n">
-        <v>68</v>
-      </c>
     </row>
     <row r="70" ht="12.5" customHeight="1">
-      <c r="A70" s="2" t="n">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B70" s="4" t="inlineStr">
+      <c r="C70" s="4" t="inlineStr">
         <is>
           <t>"35:57"</t>
         </is>
       </c>
-      <c r="C70" s="2" t="inlineStr">
+      <c r="D70" s="2" t="inlineStr">
         <is>
           <t>Margaret. I think you hit the nail on the head. I completely agree with everything you said and I believe that it's misleading, deceiving intimidating. Those that's the words. They use here eligible, voters from voting. I think that's criminal and should be charged criminally for people for doing that. And I also believe in the random audits of ballast, I think that should be, that would be aware a way to appease The General.</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E70" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with Margaret's points.
 2. The speaker believes it is misleading, deceiving, and intimidating to prevent eligible voters from voting.
@@ -2198,61 +2185,61 @@
 5. The speaker thinks that random audits of ballots would be a way to satisfy "The General."</t>
         </is>
       </c>
-      <c r="F70" t="n">
-        <v>69</v>
-      </c>
     </row>
     <row r="71" ht="12.5" customHeight="1">
-      <c r="A71" s="2" t="n">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B71" s="4" t="inlineStr">
+      <c r="C71" s="4" t="inlineStr">
         <is>
           <t>"35:57"</t>
         </is>
       </c>
-      <c r="C71" s="2" t="inlineStr">
+      <c r="D71" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Action who thinks or may think that something has been rigged. If you have random samplings audited, you could eliminate that.</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E71" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. An action is being discussed.
 2. This action is performed by someone who thinks or may think that something has been rigged.
 3. A solution to eliminate this suspicion is suggested.
-4. The solution is to have random samplings of the action audited.</t>
-        </is>
-      </c>
-      <c r="F71" t="n">
-        <v>70</v>
+4. The solution is to have random samplings audited.</t>
+        </is>
       </c>
     </row>
     <row r="72" ht="12.5" customHeight="1">
-      <c r="A72" s="2" t="n">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B72" s="4" t="inlineStr">
+      <c r="C72" s="4" t="inlineStr">
         <is>
           <t>"36:35"</t>
         </is>
       </c>
-      <c r="C72" s="2" t="inlineStr">
+      <c r="D72" s="2" t="inlineStr">
         <is>
           <t>Yeah, I don't think that they should that there should be, you know, people allowed to challenge people about stuff. But I do think that that it would be appropriate to have representatives from each political or each of the main political parties, be observers at the polling places. And you know, to just watch the process and make sure everything is going right and then be able to challenge the process. Not necessarily any individual people. And as far as the</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E72" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The author does not support the idea of allowing individuals to challenge other people during voting.
 2. They propose that representatives from major political parties should be present as observers at polling places.
@@ -2260,231 +2247,230 @@
 4. Observers would have the ability to challenge the voting process, but not individual people.</t>
         </is>
       </c>
-      <c r="F72" t="n">
-        <v>71</v>
-      </c>
     </row>
     <row r="73" ht="12.5" customHeight="1">
-      <c r="A73" s="2" t="n">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B73" s="4" t="inlineStr">
+      <c r="C73" s="4" t="inlineStr">
         <is>
           <t>"36:35"</t>
         </is>
       </c>
-      <c r="C73" s="2" t="inlineStr">
+      <c r="D73" s="2" t="inlineStr">
         <is>
           <t>The audits. I think that's a no-brainer. I think it should absolutely have audits all the time.</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F73" t="n">
-        <v>72</v>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="74" ht="12.5" customHeight="1">
-      <c r="A74" s="2" t="n">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B74" s="4" t="inlineStr">
+      <c r="C74" s="4" t="inlineStr">
         <is>
           <t>"37:13"</t>
         </is>
       </c>
-      <c r="C74" s="2" t="inlineStr">
+      <c r="D74" s="2" t="inlineStr">
         <is>
           <t>Yeah, I agree. Also, with what Margaret said, everything, especially the random audit. I don't see any way you lose with that.</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E74" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with an unspecified point.
 2. The speaker agrees with a statement made by Margaret.
 3. The speaker sees no way for the situation to result in a loss, given the random audit.</t>
         </is>
       </c>
-      <c r="F74" t="n">
-        <v>73</v>
-      </c>
     </row>
     <row r="75" ht="12.5" customHeight="1">
-      <c r="A75" s="2" t="n">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="n">
         <v>48790</v>
       </c>
-      <c r="B75" s="4" t="inlineStr">
+      <c r="C75" s="4" t="inlineStr">
         <is>
           <t>"37:13"</t>
         </is>
       </c>
-      <c r="C75" s="2" t="inlineStr">
+      <c r="D75" s="2" t="inlineStr">
         <is>
           <t>Implementing that.</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F75" t="n">
-        <v>74</v>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="76" ht="12.5" customHeight="1">
-      <c r="A76" s="2" t="n">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B76" s="4" t="inlineStr">
+      <c r="C76" s="4" t="inlineStr">
         <is>
           <t>"39:09"</t>
         </is>
       </c>
-      <c r="C76" s="2" t="inlineStr">
+      <c r="D76" s="2" t="inlineStr">
         <is>
           <t>I guess I'll go first again I definitely don't like the idea of private foundations. Any private organization, what, regardless of what they are funding, anything with the election, I think would just lead to mistrust on the part of the public.</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E76" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker expresses their view on private foundations.
 2. They state that they don't like the idea of private foundations.
-3. They give their opinion on private organizations funding anything related to elections.
-4. They believe that it would lead to mistrust on the part of the public.</t>
-        </is>
-      </c>
-      <c r="F76" t="n">
-        <v>75</v>
+3. They give their opinion that any private organization funding anything related to elections would lead to mistrust on the part of the public.</t>
+        </is>
       </c>
     </row>
     <row r="77" ht="12.5" customHeight="1">
-      <c r="A77" s="2" t="n">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B77" s="4" t="inlineStr">
+      <c r="C77" s="4" t="inlineStr">
         <is>
           <t>"39:27"</t>
         </is>
       </c>
-      <c r="C77" s="2" t="inlineStr">
+      <c r="D77" s="2" t="inlineStr">
         <is>
           <t>I think that I'm in favor of congressional funding for the state's for the election process, and machines and make equipment and such. And I think that goes hand-in-hand with one of the topics from earlier, which was have minimal standards set by the, at the federal level, as minimum standards in each state. And I think in return the stuff federal government then gives money to eat.</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E77" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. In favor of congressional funding for the state's election process equipment.
 2. Minimal standards for elections should be set at the federal level.
 3. States would adhere to these minimum standards in return for federal government funding.</t>
         </is>
       </c>
-      <c r="F77" t="n">
-        <v>76</v>
-      </c>
     </row>
     <row r="78" ht="12.5" customHeight="1">
-      <c r="A78" s="2" t="n">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B78" s="4" t="inlineStr">
+      <c r="C78" s="4" t="inlineStr">
         <is>
           <t>"39:27"</t>
         </is>
       </c>
-      <c r="C78" s="2" t="inlineStr">
+      <c r="D78" s="2" t="inlineStr">
         <is>
           <t>Take to help subsidize.</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F78" t="n">
-        <v>77</v>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="79" ht="12.5" customHeight="1">
-      <c r="A79" s="2" t="n">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B79" s="4" t="inlineStr">
+      <c r="C79" s="4" t="inlineStr">
         <is>
           <t>"40:03"</t>
         </is>
       </c>
-      <c r="C79" s="2" t="inlineStr">
+      <c r="D79" s="2" t="inlineStr">
         <is>
           <t>Yeah, I think that's probably pretty good idea to have the congruent Congress fund the state's. But I agree though with Margaret, I don't think private companies, private individuals, even should have any business at all ever, providing funny because that's just a conflict of interest I think.</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F79" t="n">
-        <v>78</v>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="80" ht="12.5" customHeight="1">
-      <c r="A80" s="2" t="n">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B80" s="4" t="inlineStr">
+      <c r="C80" s="4" t="inlineStr">
         <is>
           <t>"40:31"</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F80" t="n">
-        <v>79</v>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="81" ht="12.5" customHeight="1">
-      <c r="A81" s="2" t="n">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B81" s="4" t="inlineStr">
+      <c r="C81" s="4" t="inlineStr">
         <is>
           <t>"40:31"</t>
         </is>
       </c>
-      <c r="C81" s="2" t="inlineStr">
+      <c r="D81" s="2" t="inlineStr">
         <is>
           <t>I'm wondering how people feel about the chief electoral officer being elected as opposed to appointed. I have very mixed feelings about that. I think it should not be a political function to run elections. So I am sort of tending toward the appointment, appointment option.</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E81" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text discusses the debate over whether the chief electoral officer should be elected or appointed.
 2. The author expresses mixed feelings about this issue.
@@ -2492,30 +2478,30 @@
 4. The author is leaning towards the appointment option for the chief electoral officer.</t>
         </is>
       </c>
-      <c r="F81" t="n">
-        <v>80</v>
-      </c>
     </row>
     <row r="82" ht="12.5" customHeight="1">
-      <c r="A82" s="2" t="n">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B82" s="4" t="inlineStr">
+      <c r="C82" s="4" t="inlineStr">
         <is>
           <t>"41:02"</t>
         </is>
       </c>
-      <c r="C82" s="2" t="inlineStr">
+      <c r="D82" s="2" t="inlineStr">
         <is>
           <t>I agree to adding more people to vote for on the ballot. I think it's just people. Oftentimes, by the time they get to the end of the ballot, they don't even know or care, who they're voting for. And if you add one more person, it just I think would get lost. However, I have a problem with it being a political person in charge of, you know, a party person in charge of the electoral process. So I'm leaning towards a nonpartisan person.</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E82" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Agrees to adding more people to vote for on the ballot.
 2. Believes that voters often don't know or care who they're voting for by the end of the ballot.
@@ -2524,242 +2510,241 @@
 5. Leaning towards a nonpartisan person to be in charge of the electoral process.</t>
         </is>
       </c>
-      <c r="F82" t="n">
-        <v>81</v>
-      </c>
     </row>
     <row r="83" ht="12.5" customHeight="1">
-      <c r="A83" s="2" t="n">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B83" s="4" t="inlineStr">
+      <c r="C83" s="4" t="inlineStr">
         <is>
           <t>"41:02"</t>
         </is>
       </c>
-      <c r="C83" s="2" t="inlineStr">
+      <c r="D83" s="2" t="inlineStr">
         <is>
           <t>Somehow selected for this position.</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F83" t="n">
-        <v>82</v>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="84" ht="12.5" customHeight="1">
-      <c r="A84" s="2" t="n">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B84" s="4" t="inlineStr">
+      <c r="C84" s="4" t="inlineStr">
         <is>
           <t>"41:35"</t>
         </is>
       </c>
-      <c r="C84" s="2" t="inlineStr">
+      <c r="D84" s="2" t="inlineStr">
         <is>
           <t>Yeah, I would want somebody nonpartisan being in charge of the elections, especially since now we have people who are running their entire campaigns on that, they don't think the elections are fair. And so, they're the ones who are going to fix the system. The waste, they see that it's been, you know, as long as it goes their way, then it's fine. But if it doesn't go their way than well, there must have been fraud.</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E84" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. A nonpartisan person should be in charge of elections.
 2. This is important because some people believe the elections are not fair.
 3. Those people are running their campaigns on the idea that the elections are not fair.
-4. They claim they will fix the system if they are elected.
-5. These people see waste in the system if it benefits their opponents.
-6. However, they claim fraud if the system does not benefit them.</t>
-        </is>
-      </c>
-      <c r="F84" t="n">
-        <v>83</v>
+4. They claim that if they lose, it must be due to fraud.
+5. These individuals are willing to fix the system only if it benefits them.
+6. The system is seen as wasteful if it does not go their way.</t>
+        </is>
       </c>
     </row>
     <row r="85" ht="12.5" customHeight="1">
-      <c r="A85" s="2" t="n">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="2" t="n">
         <v>48621</v>
       </c>
-      <c r="B85" s="4" t="inlineStr">
+      <c r="C85" s="4" t="inlineStr">
         <is>
           <t>"41:35"</t>
         </is>
       </c>
-      <c r="C85" s="2" t="inlineStr">
+      <c r="D85" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> So yeah, I would not want those people no matter what party they were in being in charge of the elections.</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E85" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text expresses the speaker's opinion about certain people.
 2. The speaker does not want these people to be in charge of elections.
 3. The speaker's objection is not related to the political party that these people are associated with.</t>
         </is>
       </c>
-      <c r="F85" t="n">
-        <v>84</v>
-      </c>
     </row>
     <row r="86" ht="12.5" customHeight="1">
-      <c r="A86" s="2" t="n">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B86" s="4" t="inlineStr">
+      <c r="C86" s="4" t="inlineStr">
         <is>
           <t>"42:13"</t>
         </is>
       </c>
-      <c r="C86" s="2" t="inlineStr">
+      <c r="D86" s="2" t="inlineStr">
         <is>
           <t>Yeah, I think theoretically, that makes a lot of sense to have it. Be somebody. That's nonpartisan. I am not sure how that would work considering that I think it's really tough to take partisanship out of any appointment even because who appoints the person and and all that. And and I think they even, you know, they have somebody that they report to all the time. So there's gonna be politics involved, but I think trying to</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E86" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The idea of having a nonpartisan "Be somebody" appointment is theoretically sound.
 2. It is uncertain how this would work in practice, considering the inherent partisanship in any appointment.
-3. The person making the appointment and the person being appointed will bring their own political perspectives.
-4. Even with a nonpartisan appointment, there will still be politics involved due to reporting structures and influence.
-5. The concept of a completely nonpartisan appointment is difficult to achieve in reality.</t>
-        </is>
-      </c>
-      <c r="F86" t="n">
-        <v>85</v>
+3. The person who makes the appointment and their reporting structure will likely involve politics.
+4. Despite these challenges, the concept of trying to remove partisanship from appointments is worth considering.</t>
+        </is>
       </c>
     </row>
     <row r="87" ht="12.5" customHeight="1">
-      <c r="A87" s="2" t="n">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="2" t="n">
         <v>48846</v>
       </c>
-      <c r="B87" s="4" t="inlineStr">
+      <c r="C87" s="4" t="inlineStr">
         <is>
           <t>"42:13"</t>
         </is>
       </c>
-      <c r="C87" s="2" t="inlineStr">
+      <c r="D87" s="2" t="inlineStr">
         <is>
           <t>to get out of it as much as possible to be better.</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F87" t="n">
-        <v>86</v>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="88" ht="12.5" customHeight="1">
-      <c r="A88" s="2" t="n">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="2" t="n">
         <v>48651</v>
       </c>
-      <c r="B88" s="4" t="inlineStr">
+      <c r="C88" s="4" t="inlineStr">
         <is>
           <t>"45:41"</t>
         </is>
       </c>
-      <c r="C88" s="2" t="inlineStr">
+      <c r="D88" s="2" t="inlineStr">
         <is>
           <t>I guess nobody has any questions this time.</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F88" t="n">
-        <v>87</v>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="89" ht="12.5" customHeight="1">
-      <c r="A89" s="2" t="n">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B89" s="4" t="inlineStr">
+      <c r="C89" s="4" t="inlineStr">
         <is>
           <t>"45:47"</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F89" t="n">
-        <v>88</v>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="90" ht="12.5" customHeight="1">
-      <c r="A90" s="2" t="n">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B90" s="4" t="inlineStr">
+      <c r="C90" s="4" t="inlineStr">
         <is>
           <t>"45:47"</t>
         </is>
       </c>
-      <c r="C90" s="2" t="inlineStr">
+      <c r="D90" s="2" t="inlineStr">
         <is>
           <t>Yeah, I think there were just too many topics too much territory covered in Too Short a time and I just I don't know, I didn't get too excited about anything.</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E90" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text mentions that there were many topics covered.
 2. The speaker felt that there was too much ground covered in too short a time.
 3. The speaker did not feel excited about anything in particular.</t>
         </is>
       </c>
-      <c r="F90" t="n">
-        <v>89</v>
-      </c>
     </row>
     <row r="91" ht="12.5" customHeight="1">
-      <c r="A91" s="2" t="n">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="2" t="n">
         <v>48614</v>
       </c>
-      <c r="B91" s="4" t="inlineStr">
+      <c r="C91" s="4" t="inlineStr">
         <is>
           <t>"45:59"</t>
         </is>
       </c>
-      <c r="C91" s="2" t="inlineStr">
+      <c r="D91" s="2" t="inlineStr">
         <is>
           <t>The only question I sort of had and I'm not sure if it's worded correctly, if the federal government sets standards for registration or voting could then be challenged legally or overturned by the Supreme Court.</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
       <c r="E91" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The federal government sets standards for registration or voting.
 2. This action could be challenged legally.
@@ -2767,165 +2752,45 @@
 4. The Supreme Court would be the entity to overturn these standards.</t>
         </is>
       </c>
-      <c r="F91" t="n">
-        <v>90</v>
-      </c>
     </row>
     <row r="92" ht="12.5" customHeight="1">
-      <c r="A92" s="2" t="n">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B92" s="4" t="inlineStr">
+      <c r="C92" s="4" t="inlineStr">
         <is>
           <t>"46:27"</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F92" t="n">
-        <v>91</v>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
     </row>
     <row r="93" ht="12.5" customHeight="1">
-      <c r="A93" s="2" t="n">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="2" t="n">
         <v>48674</v>
       </c>
-      <c r="B93" s="4" t="inlineStr">
+      <c r="C93" s="4" t="inlineStr">
         <is>
           <t>"46:27"</t>
         </is>
       </c>
-      <c r="C93" s="2" t="inlineStr">
+      <c r="D93" s="2" t="inlineStr">
         <is>
           <t>I think it's too late to get anything in now.</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F93" t="n">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.5"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>proposal</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="14.5" customHeight="1">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Implement RCV as an alternative method both to elected officials and representatives at all levels</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="14.5" customHeight="1">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>Change the primary system</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="14.5" customHeight="1">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>Use proportional representatives to elect elected officials</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="14.5" customHeight="1">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>Change the current electoral college</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="14.5" customHeight="1">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>Implement more accessibility to voting</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="14.5" customHeight="1">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Restore federal and state voting rights to citizens with felony convictions upon their release from prison</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="14.5" customHeight="1">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Implement voting standards that are less strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="14.5" customHeight="1">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Implement more measures to address voter fraud</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="14.5" customHeight="1">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>Implement more fairness and transparency in the election process</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="14.5" customHeight="1">
-      <c r="A11" s="5" t="inlineStr">
-        <is>
-          <t>Implement limits on financing individual candidates and parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="14.5" customHeight="1">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>Increase in public funding and financing for campaigns</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="14.5" customHeight="1">
-      <c r="A13" s="5" t="inlineStr">
-        <is>
-          <t>Implement a term limit for Supreme Court Justices</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="14.5" customHeight="1">
-      <c r="A14" s="5" t="inlineStr">
-        <is>
-          <t>Increase opportunities for learning about civic education in schools</t>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code cleanup and test run
</commit_message>
<xml_diff>
--- a/processing/test/20230613-a1r-nc-session3-g_transcript.xlsx
+++ b/processing/test/20230613-a1r-nc-session3-g_transcript.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20230613-a1r-nc-session3-g_tran" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="in" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -61,7 +61,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -72,6 +72,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,244 +361,257 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="12.6328125" customWidth="1" style="3" min="1" max="1"/>
-    <col width="12.6328125" customWidth="1" style="3" min="3" max="4"/>
+    <col width="12.5" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.5" customWidth="1" min="2" max="2"/>
+    <col width="13.5" customWidth="1" style="3" min="3" max="4"/>
+    <col width="246.5" customWidth="1" min="4" max="4"/>
+    <col width="16.5" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Order</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>speaker</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Speaker</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Has Arguments</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>All Arguments Summarized</t>
         </is>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="n">
+      <c r="A2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>"2:04"</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>This is Jim in Buffalo New York.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F2" s="6" t="n"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="n">
+      <c r="A3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>"2:09"</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
         <is>
           <t>This is Margaret in Michigan.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F3" s="6" t="n"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="n">
+      <c r="A4" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="6" t="n">
         <v>48659</v>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>"2:14"</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
         <is>
           <t>Hey, this is Mark in Maine.</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="n"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="n">
+      <c r="A5" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>"2:17"</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>It says Aaron from Michigan.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="n"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" t="n">
+      <c r="A6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>"2:21"</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>And Kerry from Maryland.</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="n"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="n">
+      <c r="A7" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>"2:25"</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>Rich from Connecticut. Hopefully you can hear me. Can you hear me?</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="n"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="n">
+      <c r="A8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>"2:30"</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr">
         <is>
           <t>Yep. Yep, we can hear you Peter and Wisconsin.</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F8" s="6" t="n"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="n">
+      <c r="A9" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>"11:00"</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D9" s="6" t="n"/>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F9" s="6" t="n"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" t="n">
+      <c r="A10" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>"11:00"</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
         <is>
           <t>In particular, I like the automatic voter registration. I think that that a lot of time is wasted in in just signing people up to vote. I think the emphasis should be on the actual voting not and we have good records, you know, good motor vehicle records and other records that we can use to create these lists and that's just a starting point for their form.</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person likes automatic voter registration.
 2. They believe that a lot of time is wasted on signing people up to vote.
@@ -606,199 +622,205 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="n">
+      <c r="A11" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>"11:00"</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
         <is>
           <t>Voting. I think that's the way to go.</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F11" s="6" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" t="n">
+      <c r="A12" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>"11:38"</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
         <is>
           <t>I have a difficulty with that. I just think there's too many lists too many ways of cross-contamination and who really determines who an eligible voter is.</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E12" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F12" s="6" t="n"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" t="n">
+      <c r="A13" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>"11:55"</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
         <is>
           <t>Everybody is eligible to vote if they're over 21 pretty much, you know, unless you've got laws like you know, not allowing former felons to vote which we'll get to later. But I don't I don't really see the problem there. I mean, if there's worries about fraud that can be handled in the election process, we I think we waste a lot of time if we require people to</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F13" s="6" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" t="n">
+      <c r="A14" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>"11:55"</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>to keep registering to vote as a separate.</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F14" s="6" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" t="n">
+      <c r="A15" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="C15" s="6" t="inlineStr">
         <is>
           <t>"12:31"</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="D15" s="6" t="inlineStr">
         <is>
           <t>My question would be, how do you think we can handle the fraud in the election process?</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="E15" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F15" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Firstly, implementing a secure voter identification system to prevent voter impersonation.
-2. Secondly, ensuring the accuracy of voter registration lists to prevent duplicate or fraudulent registrations.
-3. Thirdly, monitoring and regulating campaign financing to prevent illegal or unethical influence.
-4. Additionally, establishing post-election audits to verify the results and detect any discrepancies.
-5. Furthermore, enacting strict penalties for election fraud to deter potential violators.
-6. Lastly, promoting transparency and public participation in the election process to increase accountability and trust.</t>
+2. Secondly, ensuring the transparency and accuracy of vote counting through technology and human oversight.
+3. Thirdly, establishing strict penalties for election fraud and enforcing them consistently.
+4. Additionally, promoting public education about the importance of ethical voting behavior.
+5. Furthermore, encouraging the involvement of independent observers in the election process.
+6. Lastly, regularly auditing and monitoring the election process to detect and prevent fraudulent activities.</t>
         </is>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" t="n">
+      <c r="A16" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="C16" s="6" t="inlineStr">
         <is>
           <t>"12:40"</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="D16" s="6" t="inlineStr">
         <is>
           <t>How do we handle it in the registration process?</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E16" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F16" s="6" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" t="n">
+      <c r="A17" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" s="6" t="inlineStr">
         <is>
           <t>"12:53"</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="D17" s="6" t="inlineStr">
         <is>
           <t>I agree with Peter. I think it's a would be more more uniform to just do it that way, and give people the option to opt-out certain animal with the mechanism would be to regulate, you know, who's koala a qualified voter or not. But</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F17" s="6" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" t="n">
+      <c r="A18" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C18" s="4" t="inlineStr">
+      <c r="C18" s="6" t="inlineStr">
         <is>
           <t>"13:12"</t>
         </is>
       </c>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="D18" s="6" t="inlineStr">
         <is>
           <t>I'm not against the proposal, I just see a lot of hurdles to really implementing it.</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="E18" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F18" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person does not oppose the proposal.
 2. There are many challenges or obstacles to implementing the proposal.</t>
@@ -806,77 +828,80 @@
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" t="n">
+      <c r="A19" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="6" t="n">
         <v>9671</v>
       </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="C19" s="6" t="inlineStr">
         <is>
           <t>"13:26"</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D19" s="6" t="n"/>
+      <c r="E19" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F19" s="6" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" t="n">
+      <c r="A20" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="6" t="n">
         <v>9671</v>
       </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="C20" s="6" t="inlineStr">
         <is>
           <t>"13:26"</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr">
+      <c r="D20" s="6" t="inlineStr">
         <is>
           <t>I agree with Margaret, I think it'll be just a lot of to go through and then plus you</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> have to do the analysis afterwards. Also, I don't think we have the necessary data to make informed decisions. Here are the points I agree with Margaret on:
-1. The process of going through all the data will be time-consuming.
-2. Analysis of the data will be required after collecting it.
-3. The necessary data for making informed decisions is currently lacking.</t>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F20" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> have to do the analysis afterwards. Also, I don't think we have enough information to make an informed decision. Plus, there are other factors to consider, like the time and resources it would take to implement the change.
+1. There is agreement that the process would require a lot of effort.
+2. Analysis would be required after going through the process.
+3. The reader feels there is not enough information to make an informed decision.
+4. Time and resources required for implementation are mentioned as factors to consider.</t>
         </is>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" t="n">
+      <c r="A21" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C21" s="4" t="inlineStr">
+      <c r="C21" s="6" t="inlineStr">
         <is>
           <t>"14:13"</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr">
+      <c r="D21" s="6" t="inlineStr">
         <is>
           <t>One of the other things was gloating online which I, I certainly think that that's probably not workable. I don't know what other people think about that, but I would be against</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F21" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text discusses the issue of gloating online.
 2. The author expresses their personal opinion that gloating online is not productive or workable.
@@ -886,28 +911,28 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" t="n">
+      <c r="A22" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C22" s="4" t="inlineStr">
+      <c r="C22" s="6" t="inlineStr">
         <is>
           <t>"14:29"</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr">
+      <c r="D22" s="6" t="inlineStr">
         <is>
           <t>I agree. I think that right now, there's just too many possibilities of people not knowing how to use the computer system to vote correctly, fraud, multiple voting. I think it's just too difficult.</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F22" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person believes that there are currently too many possibilities of people not knowing how to use the computer system to vote correctly.
 2. The person is concerned about the possibility of fraud.
@@ -917,210 +942,215 @@
       </c>
     </row>
     <row r="23" ht="12.5" customHeight="1">
-      <c r="A23" t="n">
+      <c r="A23" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C23" s="4" t="inlineStr">
+      <c r="C23" s="6" t="inlineStr">
         <is>
           <t>"14:46"</t>
         </is>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="D23" s="6" t="inlineStr">
         <is>
           <t>I think that the proposal is for registering to vote online, I don't think that they're necessarily proposing that we actually do the voting online itself. As far as that goes, I think Most states have, you know, allow you to do your driver's license to renew your drivers license and vehicles and stuff online. So if they can get that figured out, I think that they could tag the</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E23" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F23" s="6" t="n"/>
     </row>
     <row r="24" ht="12.5" customHeight="1">
-      <c r="A24" t="n">
+      <c r="A24" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C24" s="4" t="inlineStr">
+      <c r="C24" s="6" t="inlineStr">
         <is>
           <t>"14:46"</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr">
+      <c r="D24" s="6" t="inlineStr">
         <is>
           <t>Voter registration online as well as long as you have the proper IDs and all that kind of stuff.</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E24" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F24" s="6" t="n"/>
     </row>
     <row r="25" ht="12.5" customHeight="1">
-      <c r="A25" t="n">
+      <c r="A25" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C25" s="4" t="inlineStr">
+      <c r="C25" s="6" t="inlineStr">
         <is>
           <t>"15:21"</t>
         </is>
       </c>
-      <c r="D25" s="2" t="inlineStr">
+      <c r="D25" s="6" t="inlineStr">
         <is>
           <t>No I agree with Kerry. I think that you know the question here is can the register to vote online? And that's something that I think should be allowed, certainly not as the only option, but an additional option because in, you know, today's world is going to computers and there's no stopping that and you know I think to just not allow that as an option, I think is denying a basic</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E25" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F25" s="6" t="n"/>
     </row>
     <row r="26" ht="12.5" customHeight="1">
-      <c r="A26" t="n">
+      <c r="A26" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C26" s="4" t="inlineStr">
+      <c r="C26" s="6" t="inlineStr">
         <is>
           <t>"15:21"</t>
         </is>
       </c>
-      <c r="D26" s="2" t="inlineStr">
+      <c r="D26" s="6" t="inlineStr">
         <is>
           <t>Practice that just makes sense in today's world.</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E26" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F26" s="6" t="n"/>
     </row>
     <row r="27" ht="12.5" customHeight="1">
-      <c r="A27" t="n">
+      <c r="A27" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C27" s="4" t="inlineStr">
+      <c r="C27" s="6" t="inlineStr">
         <is>
           <t>"15:53"</t>
         </is>
       </c>
-      <c r="D27" s="2" t="inlineStr">
+      <c r="D27" s="6" t="inlineStr">
         <is>
           <t>Yeah, I agree. I'm sorry, I misread that in the other thing is allowing registering to vote on Election Day. We've had that in Wisconsin for a long time. I don't think there's any problem with that. I don't see a need for a pre-registration but I think the automat taking like the motor vehicle list makes the most sense because you've already identified people and I just don't see a problem.</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
+      <c r="E27" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F27" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with a previous statement.
 2. The speaker apologizes for a previous misreading.
 3. In Wisconsin, it is allowed to register to vote on Election Day.
 4. The speaker has no issue with this arrangement.
 5. The speaker does not see the need for pre-registration.
-6. The speaker thinks that using a list from the motor vehicle department for registration is sensible.
+6. The speaker thinks that using a list from the motor vehicle department for registration makes the most sense.
 7. The speaker sees no problems with using the motor vehicle list for registration.</t>
         </is>
       </c>
     </row>
     <row r="28" ht="12.5" customHeight="1">
-      <c r="A28" t="n">
+      <c r="A28" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C28" s="4" t="inlineStr">
+      <c r="C28" s="6" t="inlineStr">
         <is>
           <t>"16:25"</t>
         </is>
       </c>
-      <c r="D28" s="2" t="inlineStr">
+      <c r="D28" s="6" t="inlineStr">
         <is>
           <t>I agree. I think I'll registering online is fine and also the vehicle motor list and I think that would cover most people. However, there are a lot of people who do not drive so you'd have to try to figure out how to get those people. The other question. I have regarding this registration getting there by the date of the election versus I know in our state, we they allowed for time after the election.</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
+      <c r="E28" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F28" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. It is agreed to register online for the election.
 2. Registering the vehicle motor list is also recommended.
 3. It is noted that this might not cover all people, as some do not drive.
 4. A solution for this issue has not been proposed.
-5. There is a question regarding the deadline for registration - before or after the election.
-6. It is mentioned that in the speaker's state, registration is allowed after the election.</t>
+5. There is a question regarding the deadline for registration, whether it should be before or after the election date.
+6. It is mentioned that in some states, registration is allowed after the election.</t>
         </is>
       </c>
     </row>
     <row r="29" ht="12.5" customHeight="1">
-      <c r="A29" t="n">
+      <c r="A29" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C29" s="4" t="inlineStr">
+      <c r="C29" s="6" t="inlineStr">
         <is>
           <t>"16:25"</t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr">
+      <c r="D29" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> So, how do we feel about that?</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F29" s="6" t="n"/>
     </row>
     <row r="30" ht="12.5" customHeight="1">
-      <c r="A30" t="n">
+      <c r="A30" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C30" s="4" t="inlineStr">
+      <c r="C30" s="6" t="inlineStr">
         <is>
           <t>"19:03"</t>
         </is>
       </c>
-      <c r="D30" s="2" t="inlineStr">
+      <c r="D30" s="6" t="inlineStr">
         <is>
           <t>I apologize. I jumped ahead when I proposed my question about receiving, ballots on the day of the election versus waiting.</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
+      <c r="E30" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F30" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text discusses a point about election procedures.
 2. The author apologizes for bringing up a question about receiving ballots on the day of the election versus waiting.
@@ -1130,107 +1160,108 @@
       </c>
     </row>
     <row r="31" ht="12.5" customHeight="1">
-      <c r="A31" t="n">
+      <c r="A31" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C31" s="4" t="inlineStr">
+      <c r="C31" s="6" t="inlineStr">
         <is>
           <t>"19:28"</t>
         </is>
       </c>
-      <c r="D31" s="2" t="inlineStr">
+      <c r="D31" s="6" t="inlineStr">
         <is>
           <t>I know this might not be the most popular vote, but I believe in one of these, in the one I believe in is that voters should vote in person on Election Day unless medically, or health related reasons, prohibit them from doing that. I think that that's some I don't like the idea of mail-in ballots. I think it's a mess. It causes too many problems and it's just, it's unreliable and too easy to be manipulated.</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F31" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker believes that voters should vote in person on Election Day.
 2. The speaker thinks that mail-in ballots are not a good idea.
 3. The speaker believes that mail-in ballots cause too many problems.
 4. The speaker thinks that mail-in ballots are unreliable.
-5. The speaker believes that mail-in ballots are easy to manipulate.
-6. The speaker does not like the idea of mail-in ballots for health or medical reasons.</t>
+5. The speaker believes that mail-in ballots are easy to manipulate.</t>
         </is>
       </c>
     </row>
     <row r="32" ht="12.5" customHeight="1">
-      <c r="A32" t="n">
+      <c r="A32" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C32" s="4" t="inlineStr">
+      <c r="C32" s="6" t="inlineStr">
         <is>
           <t>"19:56"</t>
         </is>
       </c>
-      <c r="D32" s="2" t="inlineStr">
+      <c r="D32" s="6" t="inlineStr">
         <is>
           <t>Yeah, I completely disagree with that. I think I vote by mail has worked very well. And a lot of places. There are some states that do all their elections by mail and they have not really had problems. I think, I think Oregon does that. I think maybe Utah does that. And we certainly have have it available in Wisconsin. So I'm I'm really all four</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E32" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F32" s="6" t="n"/>
     </row>
     <row r="33" ht="12.5" customHeight="1">
-      <c r="A33" t="n">
+      <c r="A33" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C33" s="4" t="inlineStr">
+      <c r="C33" s="6" t="inlineStr">
         <is>
           <t>"19:56"</t>
         </is>
       </c>
-      <c r="D33" s="2" t="inlineStr">
+      <c r="D33" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Voting by mail you, I just tell you I don't think we've had a problem with it.</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F33" s="6" t="n"/>
     </row>
     <row r="34" ht="12.5" customHeight="1">
-      <c r="A34" t="n">
+      <c r="A34" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C34" s="4" t="inlineStr">
+      <c r="C34" s="6" t="inlineStr">
         <is>
           <t>"20:33"</t>
         </is>
       </c>
-      <c r="D34" s="2" t="inlineStr">
+      <c r="D34" s="6" t="inlineStr">
         <is>
           <t>I don't like that by now. I think people should be required to be in person. I also think that people should be required to show ID when they vote, which is something that you can't ask them to do with the vote by mail. However, I think there should be a couple either exceptions to people that are allowed to vote by mail because like, I know my, my son is still in college and it while it's still within the state. It's three and a half hours away. He can't make it back.</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
+      <c r="E34" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F34" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person expresses dislike towards something.
 2. They believe people should be required to vote in person.
@@ -1242,28 +1273,28 @@
       </c>
     </row>
     <row r="35" ht="12.5" customHeight="1">
-      <c r="A35" t="n">
+      <c r="A35" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C35" s="4" t="inlineStr">
+      <c r="C35" s="6" t="inlineStr">
         <is>
           <t>"20:33"</t>
         </is>
       </c>
-      <c r="D35" s="2" t="inlineStr">
+      <c r="D35" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Back to, to vote on Election Day. So he kind of has to do by mail</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
+      <c r="E35" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F35" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. A person, named John, plans to go out of town for vacation.
 2. John's vacation will coincide with the Election Day.
@@ -1272,28 +1303,28 @@
       </c>
     </row>
     <row r="36" ht="12.5" customHeight="1">
-      <c r="A36" t="n">
+      <c r="A36" s="6" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C36" s="4" t="inlineStr">
+      <c r="C36" s="6" t="inlineStr">
         <is>
           <t>"21:09"</t>
         </is>
       </c>
-      <c r="D36" s="2" t="inlineStr">
+      <c r="D36" s="6" t="inlineStr">
         <is>
           <t>Yeah, I'm fine with voting by mail. I mean, obviously this last election there are tons of audits done and everything checked out there was no evidence of fraud. I can also say I'm very much in favor of early voting because I have lived in a small town of just 2,000 people in Michigan. That I also lived in</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
+      <c r="E36" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F36" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The writer is in favor of voting by mail.
 2. In the last election, there were numerous audits done, and no evidence of fraud was found.
@@ -1303,28 +1334,28 @@
       </c>
     </row>
     <row r="37" ht="12.5" customHeight="1">
-      <c r="A37" t="n">
+      <c r="A37" s="6" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B37" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C37" s="4" t="inlineStr">
+      <c r="C37" s="6" t="inlineStr">
         <is>
           <t>"21:09"</t>
         </is>
       </c>
-      <c r="D37" s="2" t="inlineStr">
+      <c r="D37" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> In Miami, Florida. And I did early voting in Miami and I had to wait for hours to do early voting. If you wait the day of sometimes, it might be 12-hour. Wait,</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
+      <c r="E37" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F37" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The individual voted in Miami, Florida.
 2. They participated in early voting in Miami.
@@ -1334,28 +1365,28 @@
       </c>
     </row>
     <row r="38" ht="12.5" customHeight="1">
-      <c r="A38" t="n">
+      <c r="A38" s="6" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="n">
+      <c r="B38" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C38" s="4" t="inlineStr">
+      <c r="C38" s="6" t="inlineStr">
         <is>
           <t>"22:02"</t>
         </is>
       </c>
-      <c r="D38" s="2" t="inlineStr">
+      <c r="D38" s="6" t="inlineStr">
         <is>
           <t>I think we have to think of the military and people who are out of the country, for example, on business. I think those should individuals should be allowed to vote by mail. In addition, to elderly people above a certain age, the way it is now. So I'm all in favor for male voting. And I have no problem with early voting either as long as it's a reasonable amount of time within the election day.</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
+      <c r="E38" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F38" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The military and people who are outside of the country for work should be allowed to vote by mail.
 2. Elderly people, beyond a certain age, should continue to be allowed to vote in the way they do now (which may imply voting by mail for some of them).
@@ -1365,173 +1396,172 @@
       </c>
     </row>
     <row r="39" ht="12.5" customHeight="1">
-      <c r="A39" t="n">
+      <c r="A39" s="6" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="n">
+      <c r="B39" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C39" s="4" t="inlineStr">
+      <c r="C39" s="6" t="inlineStr">
         <is>
           <t>"22:39"</t>
         </is>
       </c>
-      <c r="D39" s="2" t="inlineStr">
+      <c r="D39" s="6" t="inlineStr">
         <is>
           <t>What do you think about the video cameras at the voting site?</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E39" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F39" s="6" t="n"/>
     </row>
     <row r="40" ht="12.5" customHeight="1">
-      <c r="A40" t="n">
+      <c r="A40" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="n">
+      <c r="B40" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C40" s="4" t="inlineStr">
+      <c r="C40" s="6" t="inlineStr">
         <is>
           <t>"22:50"</t>
         </is>
       </c>
-      <c r="D40" s="2" t="inlineStr">
+      <c r="D40" s="6" t="inlineStr">
         <is>
           <t>I don't see a problem with that, I know and some cases, I think the last election they had police officers monitoring the boxes but I don't see any problem having a camera there for security. Keep everything legit.</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E40" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F40" s="6" t="n"/>
     </row>
     <row r="41" ht="12.5" customHeight="1">
-      <c r="A41" t="n">
+      <c r="A41" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="n">
+      <c r="B41" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C41" s="4" t="inlineStr">
+      <c r="C41" s="6" t="inlineStr">
         <is>
           <t>"23:16"</t>
         </is>
       </c>
-      <c r="D41" s="2" t="inlineStr">
+      <c r="D41" s="6" t="inlineStr">
         <is>
           <t>I don't have a problem with the video cameras either as long as everybody knows about it, I do have a problem with a paper record where the voter has to verify and and then put it in. I think, just adding a layer, a confusing layer to the voting process</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1. The person mentioned does not have an issue with video cameras at polling stations, as long as their presence is known to everyone.
-2. They have a concern with a system that involves a paper record which the voter has to verify and then submit.
-3. They believe that this additional layer could make the voting process more confusing.</t>
-        </is>
-      </c>
+      <c r="E41" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F41" s="6" t="n"/>
     </row>
     <row r="42" ht="12.5" customHeight="1">
-      <c r="A42" t="n">
+      <c r="A42" s="6" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C42" s="4" t="inlineStr">
+      <c r="C42" s="6" t="inlineStr">
         <is>
           <t>"25:46"</t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr">
+      <c r="D42" s="6" t="inlineStr">
         <is>
           <t>I would be for uniform Across the Nation because otherwise, you can do get situations where in certain States, they make it more difficult for people in large cities to vote. And I can say that as somebody who lived in Florida and when I lived in Miami, you know, like I said, even doing early voting, I waited my wife and I waited for hours to vote. And then later,</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E42" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F42" s="6" t="n"/>
     </row>
     <row r="43" ht="12.5" customHeight="1">
-      <c r="A43" t="n">
+      <c r="A43" s="6" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C43" s="4" t="inlineStr">
+      <c r="C43" s="6" t="inlineStr">
         <is>
           <t>"25:46"</t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr">
+      <c r="D43" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Iran. They did things like quietly removed bathrooms out. Hoses from where people were boating basically, to try to discourage people from coming and voting.</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E43" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F43" s="6" t="n"/>
     </row>
     <row r="44" ht="12.5" customHeight="1">
-      <c r="A44" t="n">
+      <c r="A44" s="6" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C44" s="4" t="inlineStr">
+      <c r="C44" s="6" t="inlineStr">
         <is>
           <t>"26:36"</t>
         </is>
       </c>
-      <c r="D44" s="2" t="inlineStr">
+      <c r="D44" s="6" t="inlineStr">
         <is>
           <t>I'm torn on this one because they're, like I said, there are times when certain areas do things that are not acceptable, but on the other hand, I fear too much Federal level control and would that allow states to try new methods new techniques for voting like some of the different states have tried. So I'm sort of torn out on this one.</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E44" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F44" s="6" t="n"/>
     </row>
     <row r="45" ht="12.5" customHeight="1">
-      <c r="A45" t="n">
+      <c r="A45" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C45" s="4" t="inlineStr">
+      <c r="C45" s="6" t="inlineStr">
         <is>
           <t>"27:07"</t>
         </is>
       </c>
-      <c r="D45" s="2" t="inlineStr">
+      <c r="D45" s="6" t="inlineStr">
         <is>
           <t>I think you could set like standards, you know, national standards without being too terribly specific, so that implemented so that experimentation could be allowed for in certain areas. But you wouldn't have to, you know, you would have to make very, very specific rules. Just overall standards for voting.</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
+      <c r="E45" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F45" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. It is suggested to establish national standards for voting.
 2. These standards should not be too specific, to allow for experimentation in certain areas.
@@ -1540,28 +1570,28 @@
       </c>
     </row>
     <row r="46" ht="12.5" customHeight="1">
-      <c r="A46" t="n">
+      <c r="A46" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="n">
+      <c r="B46" s="6" t="n">
         <v>48659</v>
       </c>
-      <c r="C46" s="4" t="inlineStr">
+      <c r="C46" s="6" t="inlineStr">
         <is>
           <t>"27:37"</t>
         </is>
       </c>
-      <c r="D46" s="2" t="inlineStr">
+      <c r="D46" s="6" t="inlineStr">
         <is>
           <t>yeah, kind of along the lines with Peter was saying, I don't necessarily think that should be uniform, standards Nationwide, but I think there should be minimum standards for each of the different aspects of mail-in voting early finger on Election Day voting that at least keep working minimum standards</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
+      <c r="E46" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F46" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with Peter's viewpoint.
 2. The speaker does not believe that voting standards should be uniform nationwide.
@@ -1570,223 +1600,223 @@
       </c>
     </row>
     <row r="47" ht="12.5" customHeight="1">
-      <c r="A47" t="n">
+      <c r="A47" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="n">
+      <c r="B47" s="6" t="n">
         <v>48660</v>
       </c>
-      <c r="C47" s="4" t="inlineStr">
+      <c r="C47" s="6" t="inlineStr">
         <is>
           <t>"28:01"</t>
         </is>
       </c>
-      <c r="D47" s="2" t="inlineStr">
+      <c r="D47" s="6" t="inlineStr">
         <is>
           <t>Yeah, I agree with both Peter and Mark one of those standards would be individuals having to produce a government-issued ID at the time of voting to make sure that people are actually in fact eligible. So I think that would be one of the basic standards for</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1. The use of government-issued IDs at voting locations to verify the eligibility of individuals.
-2. This standard is supported by both Peter and Mark.
-3. It aims to ensure that people are voting legally and not committing fraud.
-4. The standard is a basic requirement for a secure and fair voting process.</t>
-        </is>
-      </c>
+      <c r="E47" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F47" s="6" t="n"/>
     </row>
     <row r="48" ht="12.5" customHeight="1">
-      <c r="A48" t="n">
+      <c r="A48" s="6" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="n">
+      <c r="B48" s="6" t="n">
         <v>48660</v>
       </c>
-      <c r="C48" s="4" t="inlineStr">
+      <c r="C48" s="6" t="inlineStr">
         <is>
           <t>"28:01"</t>
         </is>
       </c>
-      <c r="D48" s="2" t="inlineStr">
+      <c r="D48" s="6" t="inlineStr">
         <is>
           <t>voting.</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E48" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F48" s="6" t="n"/>
     </row>
     <row r="49" ht="12.5" customHeight="1">
-      <c r="A49" t="n">
+      <c r="A49" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="n">
+      <c r="B49" s="6" t="n">
         <v>48660</v>
       </c>
-      <c r="C49" s="4" t="inlineStr">
+      <c r="C49" s="6" t="inlineStr">
         <is>
           <t>"28:01"</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D49" s="6" t="n"/>
+      <c r="E49" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F49" s="6" t="n"/>
     </row>
     <row r="50" ht="12.5" customHeight="1">
-      <c r="A50" t="n">
+      <c r="A50" s="6" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="n">
+      <c r="B50" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C50" s="4" t="inlineStr">
+      <c r="C50" s="6" t="inlineStr">
         <is>
           <t>"28:27"</t>
         </is>
       </c>
-      <c r="D50" s="2" t="inlineStr">
+      <c r="D50" s="6" t="inlineStr">
         <is>
           <t>As far as ideas go, I just I'm okay with IDs having to present an 80s, but I do think that there should be a variety of ideas accepted, not all ideas are stupid. There are there have been cases? I think maybe in Texas, were they had, they were allowing like hunting licenses but not student IDs. And you know what was behind that I wonder?</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1. The speaker is open to the idea of IDs requiring a specific design from the 1980s.
-2. The speaker believes that a variety of ideas should be accepted, and not all ideas are bad.
-3. There is a reference to a potential case in Texas where hunting licenses were allowed, but not student IDs.
-4. The speaker wonders about the motivation behind this hypothetical situation.</t>
+      <c r="E50" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F50" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is open to the idea of IDs having a retro 80s design.
+2. The speaker believes that a variety of ideas should be accepted, implying that not all ideas are being considered.
+3. The speaker mentions an example of Texas allowing hunting licenses but not student IDs, suggesting that there may have been a specific reason behind this decision.
+4. The speaker wonders about the motivation or rationale behind certain decisions related to IDs.</t>
         </is>
       </c>
     </row>
     <row r="51" ht="12.5" customHeight="1">
-      <c r="A51" t="n">
+      <c r="A51" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="n">
+      <c r="B51" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C51" s="4" t="inlineStr">
+      <c r="C51" s="6" t="inlineStr">
         <is>
           <t>"29:03"</t>
         </is>
       </c>
-      <c r="D51" s="2" t="inlineStr">
+      <c r="D51" s="6" t="inlineStr">
         <is>
           <t>That's interesting, hunting licenses versus student IDs. I like the idea of basic standardized requirements and then within that each state could work out what works best for them.</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E51" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F51" s="6" t="n"/>
     </row>
     <row r="52" ht="12.5" customHeight="1">
-      <c r="A52" t="n">
+      <c r="A52" s="6" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="n">
+      <c r="B52" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C52" s="4" t="inlineStr">
+      <c r="C52" s="6" t="inlineStr">
         <is>
           <t>"29:23"</t>
         </is>
       </c>
-      <c r="D52" s="2" t="inlineStr">
+      <c r="D52" s="6" t="inlineStr">
         <is>
           <t>I agree standardized requirements would work as far as the IDS, I'm not sure maybe driver's license and then there was a don't drive a state issued ID. I'm not sure how regulated other licenses are going to be a hunting license. If that's something that's issued at a</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E52" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F52" s="6" t="n"/>
     </row>
     <row r="53" ht="12.5" customHeight="1">
-      <c r="A53" t="n">
+      <c r="A53" s="6" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="n">
+      <c r="B53" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C53" s="4" t="inlineStr">
+      <c r="C53" s="6" t="inlineStr">
         <is>
           <t>"29:23"</t>
         </is>
       </c>
-      <c r="D53" s="2" t="inlineStr">
+      <c r="D53" s="6" t="inlineStr">
         <is>
           <t>Sporting good store or something like that is.</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E53" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F53" s="6" t="n"/>
     </row>
     <row r="54" ht="12.5" customHeight="1">
-      <c r="A54" t="n">
+      <c r="A54" s="6" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="n">
+      <c r="B54" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C54" s="4" t="inlineStr">
+      <c r="C54" s="6" t="inlineStr">
         <is>
           <t>"29:23"</t>
         </is>
       </c>
-      <c r="D54" s="2" t="inlineStr">
+      <c r="D54" s="6" t="inlineStr">
         <is>
           <t>Is scrutinized.</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E54" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F54" s="6" t="n"/>
     </row>
     <row r="55" ht="12.5" customHeight="1">
-      <c r="A55" t="n">
+      <c r="A55" s="6" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="2" t="n">
+      <c r="B55" s="6" t="n">
         <v>9671</v>
       </c>
-      <c r="C55" s="4" t="inlineStr">
+      <c r="C55" s="6" t="inlineStr">
         <is>
           <t>"29:47"</t>
         </is>
       </c>
-      <c r="D55" s="2" t="inlineStr">
+      <c r="D55" s="6" t="inlineStr">
         <is>
           <t>Each state Most states have my line of Georgia for sure. Does, they'll give you a state issued ID for free just so you can vote and that would cut a lot of the problem with IDs down. So it'd be a state issued ID or a driver's license.</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
+      <c r="E55" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F55" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Most states require voters to show an ID
 2. Georgia is an example of a state that requires an ID to vote
@@ -1797,115 +1827,120 @@
       </c>
     </row>
     <row r="56" ht="12.5" customHeight="1">
-      <c r="A56" t="n">
+      <c r="A56" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="n">
+      <c r="B56" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C56" s="4" t="inlineStr">
+      <c r="C56" s="6" t="inlineStr">
         <is>
           <t>"30:11"</t>
         </is>
       </c>
-      <c r="D56" s="2" t="inlineStr">
+      <c r="D56" s="6" t="inlineStr">
         <is>
           <t>That's what Michigan does. Also, if you don't drive, you can go in and get a state ID, which is used for identification and almost every venue that will looks up to driver's license.</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E56" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F56" s="6" t="n"/>
     </row>
     <row r="57" ht="12.5" customHeight="1">
-      <c r="A57" t="n">
+      <c r="A57" s="6" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="2" t="n">
+      <c r="B57" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C57" s="4" t="inlineStr">
+      <c r="C57" s="6" t="inlineStr">
         <is>
           <t>"30:55"</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D57" s="6" t="n"/>
+      <c r="E57" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F57" s="6" t="n"/>
     </row>
     <row r="58" ht="12.5" customHeight="1">
-      <c r="A58" t="n">
+      <c r="A58" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="2" t="n">
+      <c r="B58" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C58" s="4" t="inlineStr">
+      <c r="C58" s="6" t="inlineStr">
         <is>
           <t>"30:55"</t>
         </is>
       </c>
-      <c r="D58" s="2" t="inlineStr">
+      <c r="D58" s="6" t="inlineStr">
         <is>
           <t>I think once a person has paid their debt to society, they ought to be able to vote. There's no question in my mind about that, I think it's terrible. That some states are not allowing former felons to</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E58" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F58" s="6" t="n"/>
     </row>
     <row r="59" ht="12.5" customHeight="1">
-      <c r="A59" t="n">
+      <c r="A59" s="6" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="2" t="n">
+      <c r="B59" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C59" s="4" t="inlineStr">
+      <c r="C59" s="6" t="inlineStr">
         <is>
           <t>"31:14"</t>
         </is>
       </c>
-      <c r="D59" s="2" t="inlineStr">
+      <c r="D59" s="6" t="inlineStr">
         <is>
           <t>I can't, I completely agree with Peter. I think you paid your debt to society. You paid the penalty your time. Now you should be able to vote. Again, is one of your rights that you earned back by doing your time.</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E59" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F59" s="6" t="n"/>
     </row>
     <row r="60" ht="12.5" customHeight="1">
-      <c r="A60" t="n">
+      <c r="A60" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="2" t="n">
+      <c r="B60" s="6" t="n">
         <v>48660</v>
       </c>
-      <c r="C60" s="4" t="inlineStr">
+      <c r="C60" s="6" t="inlineStr">
         <is>
           <t>"31:29"</t>
         </is>
       </c>
-      <c r="D60" s="2" t="inlineStr">
+      <c r="D60" s="6" t="inlineStr">
         <is>
           <t>I think the only exception to that would be if the individual was convicted and sentenced to prison. Because of voter fraud, then probably not in that case. But otherwise if we are saying that they are rehabilitated and can reenter Society, then they have a right to participate in the process of living in society. And that includes voting.</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
+      <c r="E60" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F60" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. If an individual has been convicted and sentenced to prison due to voter fraud, they probably should not be allowed to vote.
 2. Those who have been rehabilitated and can re-enter society have the right to participate in the process of living in society, including voting.</t>
@@ -1913,106 +1948,108 @@
       </c>
     </row>
     <row r="61" ht="12.5" customHeight="1">
-      <c r="A61" t="n">
+      <c r="A61" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="2" t="n">
+      <c r="B61" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C61" s="4" t="inlineStr">
+      <c r="C61" s="6" t="inlineStr">
         <is>
           <t>"31:57"</t>
         </is>
       </c>
-      <c r="D61" s="2" t="inlineStr">
+      <c r="D61" s="6" t="inlineStr">
         <is>
           <t>I agree somebody that's served their time and rehabilitated, you know, learning that right back as well.</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F61" s="6" t="n"/>
     </row>
     <row r="62" ht="12.5" customHeight="1">
-      <c r="A62" t="n">
+      <c r="A62" s="6" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="6" t="n">
         <v>9671</v>
       </c>
-      <c r="C62" s="4" t="inlineStr">
+      <c r="C62" s="6" t="inlineStr">
         <is>
           <t>"32:05"</t>
         </is>
       </c>
-      <c r="D62" s="2" t="inlineStr">
+      <c r="D62" s="6" t="inlineStr">
         <is>
           <t>I kind of disagree, I think it should go back a case-by-case bright basis. I think you should have to make some kind of requirement to do that because I mean, there's some people that I wouldn't care if they breathe much less vote.</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E62" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F62" s="6" t="n"/>
     </row>
     <row r="63" ht="12.5" customHeight="1">
-      <c r="A63" t="n">
+      <c r="A63" s="6" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="n">
+      <c r="B63" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C63" s="4" t="inlineStr">
+      <c r="C63" s="6" t="inlineStr">
         <is>
           <t>"32:21"</t>
         </is>
       </c>
-      <c r="D63" s="2" t="inlineStr">
+      <c r="D63" s="6" t="inlineStr">
         <is>
           <t>I don't like the word in on some of the things the things I've seen about it saying, like, like where it says non incarcerated, I think they have to completely finish their their sentence, including any parole, I need anything like that. And so, just the fact that they're not in jail anymore, I don't think should be enough. I think they need to finish parole. And, and then at that point, I think it's probably. Okay.</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
+      <c r="E63" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F63" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker does not like the use of the word "in" in certain contexts.
-2. They have concerns about the status of individuals who have served jail time.
-3. The speaker believes that these individuals should completely finish their sentence, including any parole.
-4. The mere fact that someone is not in jail anymore is not sufficient, according to the speaker.
-5. The speaker thinks that only after finishing parole should the individual be considered for any further actions.</t>
+2. They have concerns about the status of individuals who have served jail time, but have not completed parole.
+3. The speaker believes that individuals should be required to finish their sentence, including any parole, before being considered as having fully served their time.
+4. The speaker thinks that the mere fact of not being in jail anymore is not sufficient to consider someone as having fully served their sentence.
+5. The speaker believes that only after completing parole should an individual be considered as having made a sufficient transition.</t>
         </is>
       </c>
     </row>
     <row r="64" ht="12.5" customHeight="1">
-      <c r="A64" t="n">
+      <c r="A64" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="n">
+      <c r="B64" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C64" s="4" t="inlineStr">
+      <c r="C64" s="6" t="inlineStr">
         <is>
           <t>"32:49"</t>
         </is>
       </c>
-      <c r="D64" s="2" t="inlineStr">
+      <c r="D64" s="6" t="inlineStr">
         <is>
           <t>I took my thoughts were along those lines. Also finish the time that they've been sentenced to, in then parole, I think as a time where they prove that they come back into society and I think once the parole has been finished, then they should be eligible to vote.</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
+      <c r="E64" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F64" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker's thoughts align with the listener's viewpoint.
 2. The speaker believes that a person's sentence should include a parole period.
@@ -2022,46 +2059,48 @@
       </c>
     </row>
     <row r="65" ht="12.5" customHeight="1">
-      <c r="A65" t="n">
+      <c r="A65" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="n">
+      <c r="B65" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C65" s="4" t="inlineStr">
+      <c r="C65" s="6" t="inlineStr">
         <is>
           <t>"34:35"</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D65" s="6" t="n"/>
+      <c r="E65" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F65" s="6" t="n"/>
     </row>
     <row r="66" ht="12.5" customHeight="1">
-      <c r="A66" t="n">
+      <c r="A66" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="n">
+      <c r="B66" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C66" s="4" t="inlineStr">
+      <c r="C66" s="6" t="inlineStr">
         <is>
           <t>"34:35"</t>
         </is>
       </c>
-      <c r="D66" s="2" t="inlineStr">
+      <c r="D66" s="6" t="inlineStr">
         <is>
           <t>I am very much against having people just random people challenging voters. I think that's intimidating, and I don't think that should be done. I think that, you know, having voter ID and all that sort of thing, you know, is the way of legitimizing Voters, and not having just people show up at the polls and and challenging people that they, they think.</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
+      <c r="E66" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F66" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker is against having random people challenging voters.
 2. The speaker finds this practice intimidating.
@@ -2071,82 +2110,85 @@
       </c>
     </row>
     <row r="67" ht="12.5" customHeight="1">
-      <c r="A67" t="n">
+      <c r="A67" s="6" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="n">
+      <c r="B67" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C67" s="4" t="inlineStr">
+      <c r="C67" s="6" t="inlineStr">
         <is>
           <t>"34:35"</t>
         </is>
       </c>
-      <c r="D67" s="2" t="inlineStr">
+      <c r="D67" s="6" t="inlineStr">
         <is>
           <t>Might have voted the way they didn't like or whatever. I just think that's a terrible idea.</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E67" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F67" s="6" t="n"/>
     </row>
     <row r="68" ht="12.5" customHeight="1">
-      <c r="A68" t="n">
+      <c r="A68" s="6" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="2" t="n">
+      <c r="B68" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C68" s="4" t="inlineStr">
+      <c r="C68" s="6" t="inlineStr">
         <is>
           <t>"35:11"</t>
         </is>
       </c>
-      <c r="D68" s="2" t="inlineStr">
+      <c r="D68" s="6" t="inlineStr">
         <is>
           <t>I agree. I agree with that. I think, like you said, it's intimidating and unnecessary and I thought we already had criminal penalties for misleading, citizens, etc, etc. I do like the idea of random Audits and different voting areas throughout the election process. I think that would help answer some questions of people being suspicious of the process.</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1. The reader agrees that the process described is intimidating and unnecessary.
-2. The reader thinks that criminal penalties for misleading citizens already exist.
-3. The reader supports the idea of random audits during the election process.
-4. The reader believes that different voting areas throughout the election process would help address suspicions of the public regarding the process.</t>
+      <c r="E68" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F68" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker agrees with the previous statement.
+2. They find the subject matter intimidating and unnecessary.
+3. The speaker believes there are already criminal penalties for misleading citizens.
+4. The speaker appreciates the idea of random audits during the election process.
+5. They also like the idea of having different voting areas throughout the election process.
+6. The speaker thinks these ideas would help address suspicions about the process.</t>
         </is>
       </c>
     </row>
     <row r="69" ht="12.5" customHeight="1">
-      <c r="A69" t="n">
+      <c r="A69" s="6" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="2" t="n">
+      <c r="B69" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C69" s="4" t="inlineStr">
+      <c r="C69" s="6" t="inlineStr">
         <is>
           <t>"35:42"</t>
         </is>
       </c>
-      <c r="D69" s="2" t="inlineStr">
+      <c r="D69" s="6" t="inlineStr">
         <is>
           <t>Yeah, I'm very much against challenging voters. It's as to whether they're eligible or not, that's just intimidation.</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
+      <c r="E69" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F69" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The person is against challenging voters.
 2. They believe that checking eligibility is separate from challenging voters.
@@ -2155,28 +2197,28 @@
       </c>
     </row>
     <row r="70" ht="12.5" customHeight="1">
-      <c r="A70" t="n">
+      <c r="A70" s="6" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="2" t="n">
+      <c r="B70" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C70" s="4" t="inlineStr">
+      <c r="C70" s="6" t="inlineStr">
         <is>
           <t>"35:57"</t>
         </is>
       </c>
-      <c r="D70" s="2" t="inlineStr">
+      <c r="D70" s="6" t="inlineStr">
         <is>
           <t>Margaret. I think you hit the nail on the head. I completely agree with everything you said and I believe that it's misleading, deceiving intimidating. Those that's the words. They use here eligible, voters from voting. I think that's criminal and should be charged criminally for people for doing that. And I also believe in the random audits of ballast, I think that should be, that would be aware a way to appease The General.</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
+      <c r="E70" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F70" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with Margaret's points.
 2. The speaker believes it is misleading, deceiving, and intimidating to prevent eligible voters from voting.
@@ -2187,28 +2229,28 @@
       </c>
     </row>
     <row r="71" ht="12.5" customHeight="1">
-      <c r="A71" t="n">
+      <c r="A71" s="6" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="2" t="n">
+      <c r="B71" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C71" s="4" t="inlineStr">
+      <c r="C71" s="6" t="inlineStr">
         <is>
           <t>"35:57"</t>
         </is>
       </c>
-      <c r="D71" s="2" t="inlineStr">
+      <c r="D71" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Action who thinks or may think that something has been rigged. If you have random samplings audited, you could eliminate that.</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
+      <c r="E71" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F71" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. An action is being discussed.
 2. This action is performed by someone who thinks or may think that something has been rigged.
@@ -2218,28 +2260,28 @@
       </c>
     </row>
     <row r="72" ht="12.5" customHeight="1">
-      <c r="A72" t="n">
+      <c r="A72" s="6" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="2" t="n">
+      <c r="B72" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C72" s="4" t="inlineStr">
+      <c r="C72" s="6" t="inlineStr">
         <is>
           <t>"36:35"</t>
         </is>
       </c>
-      <c r="D72" s="2" t="inlineStr">
+      <c r="D72" s="6" t="inlineStr">
         <is>
           <t>Yeah, I don't think that they should that there should be, you know, people allowed to challenge people about stuff. But I do think that that it would be appropriate to have representatives from each political or each of the main political parties, be observers at the polling places. And you know, to just watch the process and make sure everything is going right and then be able to challenge the process. Not necessarily any individual people. And as far as the</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
+      <c r="E72" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F72" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The author does not support the idea of allowing individuals to challenge other people during voting.
 2. They propose that representatives from major political parties should be present as observers at polling places.
@@ -2249,51 +2291,52 @@
       </c>
     </row>
     <row r="73" ht="12.5" customHeight="1">
-      <c r="A73" t="n">
+      <c r="A73" s="6" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="2" t="n">
+      <c r="B73" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C73" s="4" t="inlineStr">
+      <c r="C73" s="6" t="inlineStr">
         <is>
           <t>"36:35"</t>
         </is>
       </c>
-      <c r="D73" s="2" t="inlineStr">
+      <c r="D73" s="6" t="inlineStr">
         <is>
           <t>The audits. I think that's a no-brainer. I think it should absolutely have audits all the time.</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E73" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F73" s="6" t="n"/>
     </row>
     <row r="74" ht="12.5" customHeight="1">
-      <c r="A74" t="n">
+      <c r="A74" s="6" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="2" t="n">
+      <c r="B74" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C74" s="4" t="inlineStr">
+      <c r="C74" s="6" t="inlineStr">
         <is>
           <t>"37:13"</t>
         </is>
       </c>
-      <c r="D74" s="2" t="inlineStr">
+      <c r="D74" s="6" t="inlineStr">
         <is>
           <t>Yeah, I agree. Also, with what Margaret said, everything, especially the random audit. I don't see any way you lose with that.</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
+      <c r="E74" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F74" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker agrees with an unspecified point.
 2. The speaker agrees with a statement made by Margaret.
@@ -2302,51 +2345,52 @@
       </c>
     </row>
     <row r="75" ht="12.5" customHeight="1">
-      <c r="A75" t="n">
+      <c r="A75" s="6" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="2" t="n">
+      <c r="B75" s="6" t="n">
         <v>48790</v>
       </c>
-      <c r="C75" s="4" t="inlineStr">
+      <c r="C75" s="6" t="inlineStr">
         <is>
           <t>"37:13"</t>
         </is>
       </c>
-      <c r="D75" s="2" t="inlineStr">
+      <c r="D75" s="6" t="inlineStr">
         <is>
           <t>Implementing that.</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E75" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F75" s="6" t="n"/>
     </row>
     <row r="76" ht="12.5" customHeight="1">
-      <c r="A76" t="n">
+      <c r="A76" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="2" t="n">
+      <c r="B76" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C76" s="4" t="inlineStr">
+      <c r="C76" s="6" t="inlineStr">
         <is>
           <t>"39:09"</t>
         </is>
       </c>
-      <c r="D76" s="2" t="inlineStr">
+      <c r="D76" s="6" t="inlineStr">
         <is>
           <t>I guess I'll go first again I definitely don't like the idea of private foundations. Any private organization, what, regardless of what they are funding, anything with the election, I think would just lead to mistrust on the part of the public.</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
+      <c r="E76" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F76" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The speaker expresses their view on private foundations.
 2. They state that they don't like the idea of private foundations.
@@ -2355,124 +2399,129 @@
       </c>
     </row>
     <row r="77" ht="12.5" customHeight="1">
-      <c r="A77" t="n">
+      <c r="A77" s="6" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="2" t="n">
+      <c r="B77" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C77" s="4" t="inlineStr">
+      <c r="C77" s="6" t="inlineStr">
         <is>
           <t>"39:27"</t>
         </is>
       </c>
-      <c r="D77" s="2" t="inlineStr">
+      <c r="D77" s="6" t="inlineStr">
         <is>
           <t>I think that I'm in favor of congressional funding for the state's for the election process, and machines and make equipment and such. And I think that goes hand-in-hand with one of the topics from earlier, which was have minimal standards set by the, at the federal level, as minimum standards in each state. And I think in return the stuff federal government then gives money to eat.</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
+      <c r="E77" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F77" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. In favor of congressional funding for the state's election process equipment.
 2. Minimal standards for elections should be set at the federal level.
-3. States would adhere to these minimum standards in return for federal government funding.</t>
+3. These minimum standards would apply in each state.
+4. In return for the funding and minimum standards, the federal government would give money to the states.</t>
         </is>
       </c>
     </row>
     <row r="78" ht="12.5" customHeight="1">
-      <c r="A78" t="n">
+      <c r="A78" s="6" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="2" t="n">
+      <c r="B78" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C78" s="4" t="inlineStr">
+      <c r="C78" s="6" t="inlineStr">
         <is>
           <t>"39:27"</t>
         </is>
       </c>
-      <c r="D78" s="2" t="inlineStr">
+      <c r="D78" s="6" t="inlineStr">
         <is>
           <t>Take to help subsidize.</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E78" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F78" s="6" t="n"/>
     </row>
     <row r="79" ht="12.5" customHeight="1">
-      <c r="A79" t="n">
+      <c r="A79" s="6" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="2" t="n">
+      <c r="B79" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C79" s="4" t="inlineStr">
+      <c r="C79" s="6" t="inlineStr">
         <is>
           <t>"40:03"</t>
         </is>
       </c>
-      <c r="D79" s="2" t="inlineStr">
+      <c r="D79" s="6" t="inlineStr">
         <is>
           <t>Yeah, I think that's probably pretty good idea to have the congruent Congress fund the state's. But I agree though with Margaret, I don't think private companies, private individuals, even should have any business at all ever, providing funny because that's just a conflict of interest I think.</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E79" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F79" s="6" t="n"/>
     </row>
     <row r="80" ht="12.5" customHeight="1">
-      <c r="A80" t="n">
+      <c r="A80" s="6" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="2" t="n">
+      <c r="B80" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C80" s="4" t="inlineStr">
+      <c r="C80" s="6" t="inlineStr">
         <is>
           <t>"40:31"</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D80" s="6" t="n"/>
+      <c r="E80" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F80" s="6" t="n"/>
     </row>
     <row r="81" ht="12.5" customHeight="1">
-      <c r="A81" t="n">
+      <c r="A81" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="2" t="n">
+      <c r="B81" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C81" s="4" t="inlineStr">
+      <c r="C81" s="6" t="inlineStr">
         <is>
           <t>"40:31"</t>
         </is>
       </c>
-      <c r="D81" s="2" t="inlineStr">
+      <c r="D81" s="6" t="inlineStr">
         <is>
           <t>I'm wondering how people feel about the chief electoral officer being elected as opposed to appointed. I have very mixed feelings about that. I think it should not be a political function to run elections. So I am sort of tending toward the appointment, appointment option.</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1. The text discusses the debate over whether the chief electoral officer should be elected or appointed.
+      <c r="E81" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F81" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The text discusses the debate around whether the chief electoral officer should be elected or appointed.
 2. The author expresses mixed feelings about this issue.
 3. The author believes that running elections should not be a political function.
 4. The author is leaning towards the appointment option for the chief electoral officer.</t>
@@ -2480,28 +2529,28 @@
       </c>
     </row>
     <row r="82" ht="12.5" customHeight="1">
-      <c r="A82" t="n">
+      <c r="A82" s="6" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="2" t="n">
+      <c r="B82" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C82" s="4" t="inlineStr">
+      <c r="C82" s="6" t="inlineStr">
         <is>
           <t>"41:02"</t>
         </is>
       </c>
-      <c r="D82" s="2" t="inlineStr">
+      <c r="D82" s="6" t="inlineStr">
         <is>
           <t>I agree to adding more people to vote for on the ballot. I think it's just people. Oftentimes, by the time they get to the end of the ballot, they don't even know or care, who they're voting for. And if you add one more person, it just I think would get lost. However, I have a problem with it being a political person in charge of, you know, a party person in charge of the electoral process. So I'm leaning towards a nonpartisan person.</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
+      <c r="E82" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F82" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Agrees to adding more people to vote for on the ballot.
 2. Believes that voters often don't know or care who they're voting for by the end of the ballot.
@@ -2512,51 +2561,52 @@
       </c>
     </row>
     <row r="83" ht="12.5" customHeight="1">
-      <c r="A83" t="n">
+      <c r="A83" s="6" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="2" t="n">
+      <c r="B83" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C83" s="4" t="inlineStr">
+      <c r="C83" s="6" t="inlineStr">
         <is>
           <t>"41:02"</t>
         </is>
       </c>
-      <c r="D83" s="2" t="inlineStr">
+      <c r="D83" s="6" t="inlineStr">
         <is>
           <t>Somehow selected for this position.</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E83" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F83" s="6" t="n"/>
     </row>
     <row r="84" ht="12.5" customHeight="1">
-      <c r="A84" t="n">
+      <c r="A84" s="6" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="2" t="n">
+      <c r="B84" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C84" s="4" t="inlineStr">
+      <c r="C84" s="6" t="inlineStr">
         <is>
           <t>"41:35"</t>
         </is>
       </c>
-      <c r="D84" s="2" t="inlineStr">
+      <c r="D84" s="6" t="inlineStr">
         <is>
           <t>Yeah, I would want somebody nonpartisan being in charge of the elections, especially since now we have people who are running their entire campaigns on that, they don't think the elections are fair. And so, they're the ones who are going to fix the system. The waste, they see that it's been, you know, as long as it goes their way, then it's fine. But if it doesn't go their way than well, there must have been fraud.</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
+      <c r="E84" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F84" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. A nonpartisan person should be in charge of elections.
 2. This is important because some people believe the elections are not fair.
@@ -2568,28 +2618,28 @@
       </c>
     </row>
     <row r="85" ht="12.5" customHeight="1">
-      <c r="A85" t="n">
+      <c r="A85" s="6" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="2" t="n">
+      <c r="B85" s="6" t="n">
         <v>48621</v>
       </c>
-      <c r="C85" s="4" t="inlineStr">
+      <c r="C85" s="6" t="inlineStr">
         <is>
           <t>"41:35"</t>
         </is>
       </c>
-      <c r="D85" s="2" t="inlineStr">
+      <c r="D85" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> So yeah, I would not want those people no matter what party they were in being in charge of the elections.</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
+      <c r="E85" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F85" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text expresses the speaker's opinion about certain people.
 2. The speaker does not want these people to be in charge of elections.
@@ -2598,28 +2648,28 @@
       </c>
     </row>
     <row r="86" ht="12.5" customHeight="1">
-      <c r="A86" t="n">
+      <c r="A86" s="6" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="2" t="n">
+      <c r="B86" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C86" s="4" t="inlineStr">
+      <c r="C86" s="6" t="inlineStr">
         <is>
           <t>"42:13"</t>
         </is>
       </c>
-      <c r="D86" s="2" t="inlineStr">
+      <c r="D86" s="6" t="inlineStr">
         <is>
           <t>Yeah, I think theoretically, that makes a lot of sense to have it. Be somebody. That's nonpartisan. I am not sure how that would work considering that I think it's really tough to take partisanship out of any appointment even because who appoints the person and and all that. And and I think they even, you know, they have somebody that they report to all the time. So there's gonna be politics involved, but I think trying to</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
+      <c r="E86" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F86" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The idea of having a nonpartisan "Be somebody" appointment is theoretically sound.
 2. It is uncertain how this would work in practice, considering the inherent partisanship in any appointment.
@@ -2629,92 +2679,96 @@
       </c>
     </row>
     <row r="87" ht="12.5" customHeight="1">
-      <c r="A87" t="n">
+      <c r="A87" s="6" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="2" t="n">
+      <c r="B87" s="6" t="n">
         <v>48846</v>
       </c>
-      <c r="C87" s="4" t="inlineStr">
+      <c r="C87" s="6" t="inlineStr">
         <is>
           <t>"42:13"</t>
         </is>
       </c>
-      <c r="D87" s="2" t="inlineStr">
+      <c r="D87" s="6" t="inlineStr">
         <is>
           <t>to get out of it as much as possible to be better.</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E87" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F87" s="6" t="n"/>
     </row>
     <row r="88" ht="12.5" customHeight="1">
-      <c r="A88" t="n">
+      <c r="A88" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="2" t="n">
+      <c r="B88" s="6" t="n">
         <v>48651</v>
       </c>
-      <c r="C88" s="4" t="inlineStr">
+      <c r="C88" s="6" t="inlineStr">
         <is>
           <t>"45:41"</t>
         </is>
       </c>
-      <c r="D88" s="2" t="inlineStr">
+      <c r="D88" s="6" t="inlineStr">
         <is>
           <t>I guess nobody has any questions this time.</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E88" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F88" s="6" t="n"/>
     </row>
     <row r="89" ht="12.5" customHeight="1">
-      <c r="A89" t="n">
+      <c r="A89" s="6" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="2" t="n">
+      <c r="B89" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C89" s="4" t="inlineStr">
+      <c r="C89" s="6" t="inlineStr">
         <is>
           <t>"45:47"</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D89" s="6" t="n"/>
+      <c r="E89" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F89" s="6" t="n"/>
     </row>
     <row r="90" ht="12.5" customHeight="1">
-      <c r="A90" t="n">
+      <c r="A90" s="6" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="2" t="n">
+      <c r="B90" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C90" s="4" t="inlineStr">
+      <c r="C90" s="6" t="inlineStr">
         <is>
           <t>"45:47"</t>
         </is>
       </c>
-      <c r="D90" s="2" t="inlineStr">
+      <c r="D90" s="6" t="inlineStr">
         <is>
           <t>Yeah, I think there were just too many topics too much territory covered in Too Short a time and I just I don't know, I didn't get too excited about anything.</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
+      <c r="E90" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F90" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The text mentions that there were many topics covered.
 2. The speaker felt that there was too much ground covered in too short a time.
@@ -2723,28 +2777,28 @@
       </c>
     </row>
     <row r="91" ht="12.5" customHeight="1">
-      <c r="A91" t="n">
+      <c r="A91" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="2" t="n">
+      <c r="B91" s="6" t="n">
         <v>48614</v>
       </c>
-      <c r="C91" s="4" t="inlineStr">
+      <c r="C91" s="6" t="inlineStr">
         <is>
           <t>"45:59"</t>
         </is>
       </c>
-      <c r="D91" s="2" t="inlineStr">
+      <c r="D91" s="6" t="inlineStr">
         <is>
           <t>The only question I sort of had and I'm not sure if it's worded correctly, if the federal government sets standards for registration or voting could then be challenged legally or overturned by the Supreme Court.</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
+      <c r="E91" s="6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F91" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. The federal government sets standards for registration or voting.
 2. This action could be challenged legally.
@@ -2754,45 +2808,48 @@
       </c>
     </row>
     <row r="92" ht="12.5" customHeight="1">
-      <c r="A92" t="n">
+      <c r="A92" s="6" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="2" t="n">
+      <c r="B92" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C92" s="4" t="inlineStr">
+      <c r="C92" s="6" t="inlineStr">
         <is>
           <t>"46:27"</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="D92" s="6" t="n"/>
+      <c r="E92" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F92" s="6" t="n"/>
     </row>
     <row r="93" ht="12.5" customHeight="1">
-      <c r="A93" t="n">
+      <c r="A93" s="6" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="2" t="n">
+      <c r="B93" s="6" t="n">
         <v>48674</v>
       </c>
-      <c r="C93" s="4" t="inlineStr">
+      <c r="C93" s="6" t="inlineStr">
         <is>
           <t>"46:27"</t>
         </is>
       </c>
-      <c r="D93" s="2" t="inlineStr">
+      <c r="D93" s="6" t="inlineStr">
         <is>
           <t>I think it's too late to get anything in now.</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="E93" s="6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F93" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>